<commit_message>
translate NIST CSF in FR
</commit_message>
<xml_diff>
--- a/tools/nist/nist-csf-1.1.xlsx
+++ b/tools/nist/nist-csf-1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5D501F-78BA-CF4B-A1B0-7347512BA2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EA265D-4B10-3847-99FA-FA26DBB375E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="456">
   <si>
     <t xml:space="preserve">ID.AM-1 </t>
   </si>
@@ -919,9 +919,6 @@
   </si>
   <si>
     <t>NIST-CSF-1.1</t>
-  </si>
-  <si>
-    <t>National Institute of Standards and Technology - Cybersecurity Framework</t>
   </si>
   <si>
     <t>framework_ref_id</t>
@@ -995,13 +992,444 @@
   </si>
   <si>
     <t>scores</t>
+  </si>
+  <si>
+    <t>name[fr]</t>
+  </si>
+  <si>
+    <t>description[fr]</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Gestion des actifs</t>
+  </si>
+  <si>
+    <t>Développez un processus d’inventaire garantissant en permanence un recensement exhaustif de vos équipements TIC (Asset).</t>
+  </si>
+  <si>
+    <t>Inventoriez toutes les plateformes, licences et applications logicielles dans votre entreprise.</t>
+  </si>
+  <si>
+    <t>Listez tous les flux de communication et de transferts de données en interne.</t>
+  </si>
+  <si>
+    <t>Listez tous les systèmes TIC externes cruciaux pour votre entreprise.</t>
+  </si>
+  <si>
+    <t>Etablissez des priorités pour les ressources inventoriées (équipements, données, temps, personnel et applications) selon leur criticité.</t>
+  </si>
+  <si>
+    <t>Définissez clairement les rôles et les responsabilités en matière de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Environnement opérationnel</t>
+  </si>
+  <si>
+    <t>Définissez, documentez et communiquez le rôle exact de votre entreprise dans la chaîne d’approvisionnement (critique).</t>
+  </si>
+  <si>
+    <t>Identifiez et communiquez l’importance de votre entreprise en tant qu’infrastructure vitale et sa position dans le secteur critique.</t>
+  </si>
+  <si>
+    <t>Evaluez et hiérarchisez les objectifs, les tâches et les activités dans l’entreprise.</t>
+  </si>
+  <si>
+    <t>Définissez les exigences de résilience pour les activités de l'entreprise dans toutes les situations opérationnelles (par exemple pendant une prise d'otage ou une attaque, en cas de reprise, en régime nominal).</t>
+  </si>
+  <si>
+    <t>Gouvernance</t>
+  </si>
+  <si>
+    <t>Édictez une politique de sécurité informatique dans votre entreprise.</t>
+  </si>
+  <si>
+    <t>Convenir entre les responsables internes (gestion des risques par ex.) et des partenaires externes, des rôles et des responsabilités en matière de sécurité informatique.</t>
+  </si>
+  <si>
+    <t>Vérifiez que votre entreprise respecte toutes les exigences légales et réglementaires en matière de cybersécurité, y compris au niveau de la protection des données.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les cyber-risques sont bien intégrés dans la gestion des risques pour toute l’entreprise.</t>
+  </si>
+  <si>
+    <t>Évaluation des risques</t>
+  </si>
+  <si>
+    <t>Identifiez les faiblesses (techniques) de vos équipements et documentez-les.</t>
+  </si>
+  <si>
+    <t>Participez à des forums et à des réunions d’experts pour échanger des informations et être au courant des cybermenaces.</t>
+  </si>
+  <si>
+    <t>Identifiez et documentez les cybermenaces, aussi bien internes qu’externes.</t>
+  </si>
+  <si>
+    <t>Identifiez l’impact potentiel des cybermenaces sur vos activités et évaluez leur probabilité d’occurrence.</t>
+  </si>
+  <si>
+    <t>Évaluez les risques pour votre entreprise en fonction des menaces, des vulnérabilités, de l’impact (sur ses activités) et de leur probabilité d’occurrence.</t>
+  </si>
+  <si>
+    <t>Définissez les mesures à prendre immédiatement lorsqu’un risque se concrétise et fixez des priorités.</t>
+  </si>
+  <si>
+    <t>Stratégie de gestion des risques</t>
+  </si>
+  <si>
+    <t>Définissez les processus de gestion des risques, gérez-les activement et faites-les confirmer par les personnes impliquées ou les parties prenantes.</t>
+  </si>
+  <si>
+    <t>Définissez et communiquez les risques supportables pour votre entreprise.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les risques supportables sont évalués en prenant en compte l’importance de votre entreprise du fait qu’elle exploite une infrastructure critique. Prenez également en considération, dans votre analyse, les risques propres au secteur.</t>
+  </si>
+  <si>
+    <t>Gestion des risques liés à la chaine d'approvisionnement</t>
+  </si>
+  <si>
+    <t>Définissez des processus clairs pour gérer les risques liés à une perturbation dans la chaîne d’approvisionnement. Faites contrôler et valider ces processus par toutes les parties prenantes.</t>
+  </si>
+  <si>
+    <t>Identifiez les fournisseurs et les prestataires de services cruciaux pour vos systèmes, composants et services critiques à partir des processus définis ci-dessus et fixez les priorités.</t>
+  </si>
+  <si>
+    <t>Exigez de vos fournisseurs et prestataires de services qu’ils s’engagent contractuellement à développer et mettre en oeuvre des mesures appropriées pour atteindre les objectifs du processus pour gérer les risques liés à la chaîne d’approvisionnement.</t>
+  </si>
+  <si>
+    <t>Faites un suivi systématique pour vous assurer que tous vos fournisseurs et prestataires de services remplissent leurs obligations conformément aux exigences. Faites-le vérifier régulièrement par des rapports d’audit ou par les résultats des tests techniques.</t>
+  </si>
+  <si>
+    <t>Définissez avec vos fournisseurs et prestataires les processus pour réagir et récupérer après des problèmes de cybersécurité. Validez ces processus par des simulations.</t>
+  </si>
+  <si>
+    <t>Protéger</t>
+  </si>
+  <si>
+    <t>Gestion des identités, authentification et contrôle d'accès</t>
+  </si>
+  <si>
+    <t>Définissez un processus clair pour octroyer et gérer les autorisations et les données d’identification pour utilisateurs, appareils/machines et processus.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que seules les personnes autorisées ont physiquement accès aux équipements TIC. Prenez des mesures concrètes pour garantir que les ressources TIC sont protégées contre tout accès physique non autorisé.</t>
+  </si>
+  <si>
+    <t>Définissez les processus pour gérer les accès à distance.</t>
+  </si>
+  <si>
+    <t>Définissez les niveaux d’autorisation en étant le plus restrictif possible et séparez les fonctions.</t>
+  </si>
+  <si>
+    <t>Vérifiez que l’intégrité de votre réseau est protégée. Séparez votre réseau au niveau logique comme physique, si c’est nécessaire et judicieux.</t>
+  </si>
+  <si>
+    <t>N’attribuez des identités numériques qu’à des personnes ou à des processus que vous avez clairement identifiés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les utilisateurs, équipements et autres biens sont authentifés avec un niveau de sécurité (simple facteur, multi-facteur) cohérent avec le risque encouru. </t>
+  </si>
+  <si>
+    <t>Sensibilisation et formation</t>
+  </si>
+  <si>
+    <t>Veillez à ce que tous vos collaborateurs soient sensibilisés et formés en matière de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que les utilisateurs ayant des niveaux d’autorisation élevés soient conscients de leur rôle et de leurs responsabilités.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que tous les acteurs extérieurs à votre entreprise (fournisseurs, clients, partenaires) soient conscients de leur rôle et de leurs responsabilités.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que tous les cadres soient conscients de leurs rôles spécifiques et de leurs responsabilités.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que les responsables de la sécurité physique et de la sécurité informatique soient conscients de leurs rôles spécifiques et de leurs responsabilités.</t>
+  </si>
+  <si>
+    <t>Sécurité des données</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les données stockées sont protégées (contre toute atteinte ou préjudice en termes de confidentialité, d’intégrité et de disponibilité).</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les données sont protégées pendant leur transmission (contre toute atteinte ou préjudice en termes de confidentialité, d’intégrité et de disponibilité).</t>
+  </si>
+  <si>
+    <t>Veillez à ce qu’un processus formel soit défini pour votre matériel TIC afin de protéger les données lorsque des équipements sont supprimés, déplacés ou remplacés.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que vos équipements TIC aient une réserve de capacité suffisante afin que vos données soient toujours disponibles.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que des mesures appropriées sont mises en oeuvre contre les fuites de données.</t>
+  </si>
+  <si>
+    <t>Définissez un processus pour vérifier l’intégrité du micrologiciel, des systèmes d’exploitation, des logiciels d’application et des données.</t>
+  </si>
+  <si>
+    <t>Pour le développement et les tests, ayez un environnement informatique totalement indépendant des systèmes de production.</t>
+  </si>
+  <si>
+    <t>Définissez un processus pour vérifier l’intégrité du matériel utilisé.</t>
+  </si>
+  <si>
+    <t>Processus et procédures de protection de l'information</t>
+  </si>
+  <si>
+    <t>Générez une configuration standard pour l’infrastructure d’information et de communication, ainsi que pour les systèmes de contrôle industriels. Assurez-vous que cette configuration par défaut obéit aux règles usuelles de sécurité (par ex. redondance N-1, configuration minimale, etc.).</t>
+  </si>
+  <si>
+    <t>Définissez un processus « cycle de vie » pour l’utilisation des équipements TIC.</t>
+  </si>
+  <si>
+    <t>Définissez un processus pour contrôler les changements de configuration.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que des sauvegardes informatiques (backups) sont effectuées, gérées et testées régulièrement (+ qu’on peut restaurer les données sauvegardées).</t>
+  </si>
+  <si>
+    <t>Veillez à ce que toutes les exigences (réglementaires) et les directives concernant les équipements « physiques » soient respectées.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que les données soient toujours détruites selon les prescriptions.</t>
+  </si>
+  <si>
+    <t>Développez et améliorez régulièrement vos processus de sécurité informatique.</t>
+  </si>
+  <si>
+    <t>Discutez de l’efficacité des différentes technologies de protection avec vos partenaires.</t>
+  </si>
+  <si>
+    <t>Instaurez des processus pour réagir aux cyberincidents. (Incident Response-Planing, Business Continuity Management, Incident Recovery, Disaster Recovery).</t>
+  </si>
+  <si>
+    <t>Testez les plans de réaction et de récupération.</t>
+  </si>
+  <si>
+    <t>Tenez compte de la cybersécurité dès le processus de recrutement (en vérifiant les antécédents ou par des contrôles de sécurité personnels, par ex.).</t>
+  </si>
+  <si>
+    <t>Développez et mettez en oeuvre un processus pour traiter les failles repérées.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que le fonctionnement, la maintenance et les éventuelles réparations des équipements soient enregistrés et documentés (journalisation). Assurez-vous qu’elles sont effectuées rapidement et en ne recourant qu’à des moyens testés et approuvés.</t>
+  </si>
+  <si>
+    <t>Enregistrez et documentez également les travaux de maintenance de vos systèmes distants. Assurez-vous qu’aucun accès non autorisé n’est possible.</t>
+  </si>
+  <si>
+    <t>Technologie de protection</t>
+  </si>
+  <si>
+    <t>Générez et vérifiez ces fichiers régulièrement, selon les exigences et les directives.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les supports amovibles sont protégés et que leur utilisation se fait dans le strict respect des directives.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que votre système soit configuré pour toujours fonctionner, même en mode dégradé.</t>
+  </si>
+  <si>
+    <t>Assurez la protection de vos réseaux de communication et de contrôle.</t>
+  </si>
+  <si>
+    <t>Définissez des scénarios pour les différents modes de fonctionnement de vos systèmes. Par ex. : fonctionnalités en cas d’attaque, fonctionnalités pendant la phase de récupération, fonctionnalités normales pendant l’exploitation.</t>
+  </si>
+  <si>
+    <t>Détecter</t>
+  </si>
+  <si>
+    <t>Anomalies et événements</t>
+  </si>
+  <si>
+    <t>Définissez des valeurs par défaut pour les opérations réseau licites et les flux de données prévus pour les utilisateurs et les systèmes. Surveillez ces valeurs en permanence.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les incidents de cybersécurité détectés sont analysés quant à leurs objectifs et méthodes.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les informations sur les incidents de cybersécurité provenant de différentes sources et capteurs sont compilées et exploitées.</t>
+  </si>
+  <si>
+    <t>Déterminez les conséquences probables des incidents.</t>
+  </si>
+  <si>
+    <t>Définissez les valeurs limites au-delà desquelles les incidents de cybersécurité doivent générer des alertes.</t>
+  </si>
+  <si>
+    <t>Surveillance continue de la sécurité</t>
+  </si>
+  <si>
+    <t>Mettez en place une surveillance permanente du réseau pour détecter les incidents de cybersécurité potentiels.</t>
+  </si>
+  <si>
+    <t>Mettez en place une surveillance continue (monitorage) de tous les équipements et des bâtiments pour détecter les incidents de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Mettez en place un monitorage de l’utilisation des TIC par les employés pour détecter les incidents de cybersécurité potentiels.</t>
+  </si>
+  <si>
+    <t>Veillez à pouvoir détecter les maliciels.</t>
+  </si>
+  <si>
+    <t>Veillez à pouvoir détecter les maliciels sur les appareils mobiles.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les activités des prestataires de services externes sont surveillées (monitorées) pour détecter d’éventuels incidents de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Surveillez votre système en permanence pour être certain que des activités ou accès liés à des personnes, équipements ou logiciels non autorisés seront détectés.</t>
+  </si>
+  <si>
+    <t>Procédez à des tests de vulnérabilité.</t>
+  </si>
+  <si>
+    <t>Processus de détection</t>
+  </si>
+  <si>
+    <t>Définissez clairement les rôles et les responsabilités pour que tous sachent bien qui est responsable de quoi et qui a telles ou telles compétences.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les processus de détection correspondent aux exigences et conditions fixées.</t>
+  </si>
+  <si>
+    <t>Testez vos processus de détection.</t>
+  </si>
+  <si>
+    <t>Communiquez aux personnes concernées (par ex. fournisseurs, clients, partenaires, autorités) les incidents que vous avez détectés.</t>
+  </si>
+  <si>
+    <t>Améliorez en permanence vos processus de détection.</t>
+  </si>
+  <si>
+    <t>Répondre</t>
+  </si>
+  <si>
+    <t>Planification de la réponse</t>
+  </si>
+  <si>
+    <t>Assurez-vous que le plan d’intervention est correctement suivi et rapidement exécuté si un incident de cybersécurité est détecté.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que toutes les personnes connaissent leurs tâches et la marche à suivre lorsqu’elles doivent réagir à un incident de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Définissez des critères pour les communications et assurez-vous que les incidents de cybersécurité sont signalés et traités conformément à ces critères.</t>
+  </si>
+  <si>
+    <t>Partagez les informations sur les incidents de cybersécurité relevés – ainsi que les enseignements qui en découlent – selon ces critères prédéfinis.</t>
+  </si>
+  <si>
+    <t>Coordonnez-vous avec les parties prenantes selon ces critères.</t>
+  </si>
+  <si>
+    <t>Améliorez la sensibilisation aux incidents de cybersécurité grâce à des échanges réguliers avec vos partenaires.</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les alertes émanant de systèmes de détection sont prises en compte et déclenchent des enquêtes. </t>
+  </si>
+  <si>
+    <t>Veillez à pouvoir évaluer correctement l’impact d’un incident de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Effectuez une analyse technique après chaque incident.</t>
+  </si>
+  <si>
+    <t>Classez les incidents selon les exigences du plan de réaction.</t>
+  </si>
+  <si>
+    <t>Des processus sont établis pour recevoir, analyser et traiter les failles reportées à l'organisation par des sources internes et externes (par exemple lors de tests d'intrusion, via des bulletins de sécurité ou des chercheurs en sécurité).</t>
+  </si>
+  <si>
+    <t>Atténuation</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les incidents de cybersécurité peuvent être circonscrits et que vous pouvez stopper leur propagation.</t>
+  </si>
+  <si>
+    <t>Assurez-vous de pouvoir réduire l’impact des incidents de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Veillez à réduire au maximum les failles récemment découvertes ou référencez-les comme des risques acceptables.</t>
+  </si>
+  <si>
+    <t>Améliorations</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les enseignements tirés des précédents incidents de cybersécurité sont intégrés à vos plans d’intervention.</t>
+  </si>
+  <si>
+    <t>Actualisez vos stratégies de réaction.</t>
+  </si>
+  <si>
+    <t>Rétablir</t>
+  </si>
+  <si>
+    <t>Planification du rétablissement</t>
+  </si>
+  <si>
+    <t>Assurez-vous que le plan de récupération est suivi à la lettre en cas d’incident de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les enseignements tirés des précédents incidents de cybersécurité sont intégrés à vos plans de récupération.</t>
+  </si>
+  <si>
+    <t>Actualisez vos stratégies de récupération.</t>
+  </si>
+  <si>
+    <t>Anticipez les réactions du public pour ne pas dégrader la réputation de votre entreprise.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que votre entreprise retrouve vite une image positive après un incident de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Communiquez à l’interne aux parties prenantes tout ce que vous avez entrepris en matière de récupération, sans oublier les cadres et la direction.</t>
+  </si>
+  <si>
+    <t>Partiel</t>
+  </si>
+  <si>
+    <t>Informé des risques</t>
+  </si>
+  <si>
+    <t>Répétable</t>
+  </si>
+  <si>
+    <t>Adaptatif</t>
+  </si>
+  <si>
+    <t>Les pratiques de gestion des risques sont approuvées par la direction, mais ne sont peut-être pas établies comme une politique à l’échelle de l’organisation.
+Il existe une sensibilisation aux risques cybersécurité au niveau de l’organisation, mais une approche globale pour les gérer n’a pas été mise en place.</t>
+  </si>
+  <si>
+    <t>L’application de la stratégie de gestion des risques cybersécurité de l’organisation est gérée de manière ad hoc.
+La sensibilisation aux risques cybersécurité est limitée au niveau organisationnel.
+Les pratiques de gestion des risques sont approuvées par la direction, mais ne sont peut-être pas établies comme une politique à l’échelle de l’organisation.</t>
+  </si>
+  <si>
+    <t>Les pratiques de gestion des risques de l’organisation sont formellement approuvées et exprimées sous forme de politique.
+Les pratiques cybersécurité de l’organisation sont régulièrement mises à jour en fonction de l’application des processus de gestion des risques, pour répondre à l’évolution des exigences métiers ou missions, des menaces et du paysage technologique.</t>
+  </si>
+  <si>
+    <t>L’organisation dispose d’une approche à l’échelle de l’entreprise pour gérer les risques cybersécurité, en utilisant des politiques, processus et procédures informés par les risques pour traiter les événements potentiels.
+L’organisation adapte ses pratiques cybersécurité en fonction des activités passées et présentes, y compris les retours d’expérience et les indicateurs prédictifs.</t>
+  </si>
+  <si>
+    <t>National Institute of Standards and Technology - Cybersecurity Framework (CSF 1.1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1132,6 +1560,21 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1484,7 +1927,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1499,6 +1942,23 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1858,7 +2318,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1873,7 +2333,7 @@
         <v>270</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1881,7 +2341,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1913,7 +2373,7 @@
         <v>274</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>291</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1921,7 +2381,7 @@
         <v>286</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1945,12 +2405,12 @@
         <v>276</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>290</v>
@@ -1974,7 +2434,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -1982,7 +2442,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -1993,7 +2453,7 @@
         <v>278</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C16" t="s">
         <v>279</v>
@@ -2004,10 +2464,10 @@
         <v>278</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -2017,37 +2477,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="186.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="61.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="103.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -2057,8 +2526,13 @@
       <c r="D2" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="8"/>
+      <c r="F2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -2069,10 +2543,14 @@
         <v>219</v>
       </c>
       <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2080,13 +2558,16 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2094,13 +2575,16 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -2108,13 +2592,16 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -2122,13 +2609,16 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2136,13 +2626,16 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2150,11 +2643,14 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G9" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>2</v>
       </c>
@@ -2165,10 +2661,14 @@
         <v>221</v>
       </c>
       <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -2176,13 +2676,16 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G11" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2190,13 +2693,16 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G12" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -2204,13 +2710,16 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -2218,13 +2727,16 @@
       <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G14" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -2232,11 +2744,14 @@
       <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>2</v>
       </c>
@@ -2247,10 +2762,14 @@
         <v>223</v>
       </c>
       <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -2258,13 +2777,16 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G17" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -2272,13 +2794,16 @@
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G18" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -2286,13 +2811,16 @@
       <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G19" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2300,11 +2828,14 @@
       <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G20" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>2</v>
       </c>
@@ -2315,10 +2846,14 @@
         <v>228</v>
       </c>
       <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -2326,13 +2861,16 @@
       <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G22" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -2340,13 +2878,16 @@
       <c r="C23" t="s">
         <v>32</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G23" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2354,13 +2895,16 @@
       <c r="C24" t="s">
         <v>34</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G24" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -2368,13 +2912,16 @@
       <c r="C25" t="s">
         <v>36</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G25" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -2382,13 +2929,16 @@
       <c r="C26" t="s">
         <v>38</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G26" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -2396,11 +2946,14 @@
       <c r="C27" t="s">
         <v>40</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>2</v>
       </c>
@@ -2411,10 +2964,14 @@
         <v>229</v>
       </c>
       <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -2422,13 +2979,16 @@
       <c r="C29" t="s">
         <v>42</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G29" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -2436,13 +2996,16 @@
       <c r="C30" t="s">
         <v>44</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G30" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -2450,11 +3013,14 @@
       <c r="C31" t="s">
         <v>46</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G31" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>2</v>
       </c>
@@ -2465,10 +3031,14 @@
         <v>227</v>
       </c>
       <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -2476,13 +3046,16 @@
       <c r="C33" t="s">
         <v>48</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G33" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -2490,13 +3063,16 @@
       <c r="C34" t="s">
         <v>50</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G34" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -2504,13 +3080,16 @@
       <c r="C35" t="s">
         <v>52</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G35" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -2518,13 +3097,16 @@
       <c r="C36" t="s">
         <v>54</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G36" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -2532,11 +3114,14 @@
       <c r="C37" t="s">
         <v>56</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G37" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
         <v>1</v>
       </c>
@@ -2546,8 +3131,13 @@
       <c r="D38" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E38" s="8"/>
+      <c r="F38" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
         <v>2</v>
       </c>
@@ -2558,10 +3148,14 @@
         <v>233</v>
       </c>
       <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -2569,13 +3163,16 @@
       <c r="C40" t="s">
         <v>58</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G40" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -2583,13 +3180,16 @@
       <c r="C41" t="s">
         <v>60</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G41" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -2597,13 +3197,16 @@
       <c r="C42" t="s">
         <v>62</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G42" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -2611,13 +3214,16 @@
       <c r="C43" t="s">
         <v>64</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G43" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -2625,13 +3231,16 @@
       <c r="C44" t="s">
         <v>66</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G44" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -2639,13 +3248,16 @@
       <c r="C45" t="s">
         <v>68</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G45" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -2653,11 +3265,14 @@
       <c r="C46" t="s">
         <v>70</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G46" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" s="2">
         <v>2</v>
       </c>
@@ -2668,10 +3283,14 @@
         <v>235</v>
       </c>
       <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -2679,13 +3298,16 @@
       <c r="C48" t="s">
         <v>72</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G48" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -2693,13 +3315,16 @@
       <c r="C49" t="s">
         <v>74</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G49" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -2707,13 +3332,16 @@
       <c r="C50" t="s">
         <v>76</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G50" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -2721,13 +3349,16 @@
       <c r="C51" t="s">
         <v>78</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G51" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -2735,11 +3366,14 @@
       <c r="C52" t="s">
         <v>80</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G52" s="5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="2">
         <v>2</v>
       </c>
@@ -2750,10 +3384,14 @@
         <v>237</v>
       </c>
       <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -2761,13 +3399,16 @@
       <c r="C54" t="s">
         <v>82</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G54" s="5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -2775,13 +3416,16 @@
       <c r="C55" t="s">
         <v>84</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G55" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -2789,13 +3433,16 @@
       <c r="C56" t="s">
         <v>86</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G56" s="5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B57">
         <v>3</v>
@@ -2803,13 +3450,16 @@
       <c r="C57" t="s">
         <v>88</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G57" s="5" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -2817,13 +3467,16 @@
       <c r="C58" t="s">
         <v>90</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G58" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -2831,13 +3484,16 @@
       <c r="C59" t="s">
         <v>92</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G59" s="5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B60">
         <v>3</v>
@@ -2845,13 +3501,16 @@
       <c r="C60" t="s">
         <v>94</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G60" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B61">
         <v>3</v>
@@ -2859,11 +3518,14 @@
       <c r="C61" t="s">
         <v>96</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G61" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2">
         <v>2</v>
       </c>
@@ -2874,10 +3536,14 @@
         <v>243</v>
       </c>
       <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="G62" s="8"/>
+    </row>
+    <row r="63" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B63">
         <v>3</v>
@@ -2885,13 +3551,16 @@
       <c r="C63" t="s">
         <v>98</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G63" s="5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B64">
         <v>3</v>
@@ -2899,13 +3568,16 @@
       <c r="C64" t="s">
         <v>100</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G64" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B65">
         <v>3</v>
@@ -2913,13 +3585,16 @@
       <c r="C65" t="s">
         <v>102</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G65" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -2927,13 +3602,16 @@
       <c r="C66" t="s">
         <v>104</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G66" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B67">
         <v>3</v>
@@ -2941,13 +3619,16 @@
       <c r="C67" t="s">
         <v>106</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G67" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B68">
         <v>3</v>
@@ -2955,13 +3636,16 @@
       <c r="C68" t="s">
         <v>108</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G68" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B69">
         <v>3</v>
@@ -2969,13 +3653,16 @@
       <c r="C69" t="s">
         <v>110</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G69" s="5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -2983,13 +3670,16 @@
       <c r="C70" t="s">
         <v>112</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G70" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B71">
         <v>3</v>
@@ -2997,13 +3687,16 @@
       <c r="C71" t="s">
         <v>114</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G71" s="5" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B72">
         <v>3</v>
@@ -3011,13 +3704,16 @@
       <c r="C72" t="s">
         <v>116</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G72" s="5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B73">
         <v>3</v>
@@ -3025,13 +3721,16 @@
       <c r="C73" t="s">
         <v>118</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G73" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B74">
         <v>3</v>
@@ -3039,11 +3738,14 @@
       <c r="C74" t="s">
         <v>120</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G74" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="2">
         <v>2</v>
       </c>
@@ -3054,10 +3756,14 @@
         <v>244</v>
       </c>
       <c r="E75" s="6"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G75" s="8"/>
+    </row>
+    <row r="76" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B76">
         <v>3</v>
@@ -3065,13 +3771,16 @@
       <c r="C76" t="s">
         <v>122</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G76" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B77">
         <v>3</v>
@@ -3079,11 +3788,14 @@
       <c r="C77" t="s">
         <v>124</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G77" s="5" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="2">
         <v>2</v>
       </c>
@@ -3094,10 +3806,14 @@
         <v>245</v>
       </c>
       <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="G78" s="8"/>
+    </row>
+    <row r="79" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B79">
         <v>3</v>
@@ -3105,13 +3821,16 @@
       <c r="C79" t="s">
         <v>126</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G79" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B80">
         <v>3</v>
@@ -3119,13 +3838,16 @@
       <c r="C80" t="s">
         <v>128</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G80" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B81">
         <v>3</v>
@@ -3133,13 +3855,16 @@
       <c r="C81" t="s">
         <v>130</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G81" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B82">
         <v>3</v>
@@ -3147,13 +3872,16 @@
       <c r="C82" t="s">
         <v>132</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="5" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G82" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -3161,11 +3889,14 @@
       <c r="C83" t="s">
         <v>134</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G83" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B84" s="2">
         <v>1</v>
       </c>
@@ -3175,9 +3906,13 @@
       <c r="D84" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E84" s="9"/>
+      <c r="F84" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G84" s="8"/>
+    </row>
+    <row r="85" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="2">
         <v>2</v>
       </c>
@@ -3188,10 +3923,14 @@
         <v>247</v>
       </c>
       <c r="E85" s="6"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G85" s="8"/>
+    </row>
+    <row r="86" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B86">
         <v>3</v>
@@ -3199,13 +3938,16 @@
       <c r="C86" t="s">
         <v>136</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G86" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B87">
         <v>3</v>
@@ -3213,13 +3955,16 @@
       <c r="C87" t="s">
         <v>138</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G87" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B88">
         <v>3</v>
@@ -3227,13 +3972,16 @@
       <c r="C88" t="s">
         <v>140</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G88" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B89">
         <v>3</v>
@@ -3241,13 +3989,16 @@
       <c r="C89" t="s">
         <v>142</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G89" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -3255,11 +4006,14 @@
       <c r="C90" t="s">
         <v>144</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G90" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B91" s="2">
         <v>2</v>
       </c>
@@ -3270,10 +4024,14 @@
         <v>249</v>
       </c>
       <c r="E91" s="6"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="G91" s="8"/>
+    </row>
+    <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B92">
         <v>3</v>
@@ -3281,13 +4039,16 @@
       <c r="C92" t="s">
         <v>146</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G92" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B93">
         <v>3</v>
@@ -3295,13 +4056,16 @@
       <c r="C93" t="s">
         <v>148</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G93" s="5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B94">
         <v>3</v>
@@ -3309,13 +4073,16 @@
       <c r="C94" t="s">
         <v>150</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="5" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G94" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -3323,13 +4090,16 @@
       <c r="C95" t="s">
         <v>152</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="5" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G95" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B96">
         <v>3</v>
@@ -3337,13 +4107,16 @@
       <c r="C96" t="s">
         <v>154</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G96" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B97">
         <v>3</v>
@@ -3351,13 +4124,16 @@
       <c r="C97" t="s">
         <v>156</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="5" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G97" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -3365,13 +4141,16 @@
       <c r="C98" t="s">
         <v>158</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="5" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G98" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B99">
         <v>3</v>
@@ -3379,11 +4158,14 @@
       <c r="C99" t="s">
         <v>160</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="5" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G99" s="5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B100" s="2">
         <v>2</v>
       </c>
@@ -3394,10 +4176,14 @@
         <v>250</v>
       </c>
       <c r="E100" s="6"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="G100" s="8"/>
+    </row>
+    <row r="101" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B101">
         <v>3</v>
@@ -3405,13 +4191,16 @@
       <c r="C101" t="s">
         <v>162</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="5" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G101" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -3419,13 +4208,16 @@
       <c r="C102" t="s">
         <v>164</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G102" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -3433,13 +4225,16 @@
       <c r="C103" t="s">
         <v>166</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E103" s="5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G103" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -3447,13 +4242,16 @@
       <c r="C104" t="s">
         <v>168</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="5" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G104" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -3461,11 +4259,14 @@
       <c r="C105" t="s">
         <v>170</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="5" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G105" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B106" s="2">
         <v>1</v>
       </c>
@@ -3475,8 +4276,13 @@
       <c r="D106" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E106" s="8"/>
+      <c r="F106" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="G106" s="8"/>
+    </row>
+    <row r="107" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B107" s="2">
         <v>2</v>
       </c>
@@ -3487,10 +4293,14 @@
         <v>265</v>
       </c>
       <c r="E107" s="6"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="G107" s="8"/>
+    </row>
+    <row r="108" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -3498,11 +4308,14 @@
       <c r="C108" t="s">
         <v>172</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="5" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G108" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B109" s="2">
         <v>2</v>
       </c>
@@ -3513,10 +4326,14 @@
         <v>266</v>
       </c>
       <c r="E109" s="6"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G109" s="8"/>
+    </row>
+    <row r="110" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B110">
         <v>3</v>
@@ -3524,13 +4341,16 @@
       <c r="C110" t="s">
         <v>174</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="5" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G110" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -3538,13 +4358,16 @@
       <c r="C111" t="s">
         <v>176</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="5" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G111" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B112">
         <v>3</v>
@@ -3552,13 +4375,16 @@
       <c r="C112" t="s">
         <v>178</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="5" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G112" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B113">
         <v>3</v>
@@ -3566,13 +4392,16 @@
       <c r="C113" t="s">
         <v>180</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="5" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G113" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -3580,11 +4409,14 @@
       <c r="C114" t="s">
         <v>182</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="5" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G114" s="5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115"/>
       <c r="B115" s="2">
         <v>2</v>
@@ -3596,10 +4428,14 @@
         <v>264</v>
       </c>
       <c r="E115" s="6"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G115" s="8"/>
+    </row>
+    <row r="116" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -3607,13 +4443,16 @@
       <c r="C116" t="s">
         <v>184</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="5" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G116" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -3621,13 +4460,16 @@
       <c r="C117" t="s">
         <v>186</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="5" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G117" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B118">
         <v>3</v>
@@ -3635,13 +4477,16 @@
       <c r="C118" t="s">
         <v>188</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="5" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G118" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B119">
         <v>3</v>
@@ -3649,13 +4494,16 @@
       <c r="C119" t="s">
         <v>190</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E119" s="5" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G119" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B120">
         <v>3</v>
@@ -3663,11 +4511,14 @@
       <c r="C120" t="s">
         <v>192</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="5" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G120" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121"/>
       <c r="B121" s="2">
         <v>2</v>
@@ -3679,10 +4530,14 @@
         <v>267</v>
       </c>
       <c r="E121" s="6"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G121" s="8"/>
+    </row>
+    <row r="122" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B122">
         <v>3</v>
@@ -3690,13 +4545,16 @@
       <c r="C122" t="s">
         <v>194</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="5" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G122" s="5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B123">
         <v>3</v>
@@ -3704,13 +4562,16 @@
       <c r="C123" t="s">
         <v>196</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="5" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G123" s="5" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B124">
         <v>3</v>
@@ -3718,11 +4579,14 @@
       <c r="C124" t="s">
         <v>198</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="5" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G124" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125"/>
       <c r="B125" s="2">
         <v>2</v>
@@ -3734,10 +4598,14 @@
         <v>268</v>
       </c>
       <c r="E125" s="6"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="G125" s="8"/>
+    </row>
+    <row r="126" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B126">
         <v>3</v>
@@ -3745,13 +4613,16 @@
       <c r="C126" t="s">
         <v>200</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="5" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G126" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B127">
         <v>3</v>
@@ -3759,11 +4630,14 @@
       <c r="C127" t="s">
         <v>202</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="5" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G127" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128"/>
       <c r="B128" s="2">
         <v>1</v>
@@ -3774,8 +4648,13 @@
       <c r="D128" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E128" s="8"/>
+      <c r="F128" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="G128" s="8"/>
+    </row>
+    <row r="129" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129"/>
       <c r="B129" s="2">
         <v>2</v>
@@ -3787,10 +4666,14 @@
         <v>269</v>
       </c>
       <c r="E129" s="6"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G129" s="8"/>
+    </row>
+    <row r="130" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B130">
         <v>3</v>
@@ -3798,11 +4681,14 @@
       <c r="C130" t="s">
         <v>204</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="5" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G130" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131"/>
       <c r="B131" s="2">
         <v>2</v>
@@ -3814,10 +4700,14 @@
         <v>268</v>
       </c>
       <c r="E131" s="6"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="G131" s="8"/>
+    </row>
+    <row r="132" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B132">
         <v>3</v>
@@ -3825,13 +4715,16 @@
       <c r="C132" t="s">
         <v>206</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E132" s="5" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G132" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B133">
         <v>3</v>
@@ -3839,11 +4732,14 @@
       <c r="C133" t="s">
         <v>208</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G133" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134"/>
       <c r="B134" s="2">
         <v>2</v>
@@ -3855,10 +4751,14 @@
         <v>266</v>
       </c>
       <c r="E134" s="6"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G134" s="8"/>
+    </row>
+    <row r="135" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B135">
         <v>3</v>
@@ -3866,13 +4766,16 @@
       <c r="C135" t="s">
         <v>210</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E135" s="5" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G135" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B136">
         <v>3</v>
@@ -3880,13 +4783,16 @@
       <c r="C136" t="s">
         <v>212</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E136" s="5" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G136" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B137">
         <v>3</v>
@@ -3894,20 +4800,20 @@
       <c r="C137" t="s">
         <v>214</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E137" s="5" t="s">
         <v>215</v>
+      </c>
+      <c r="G137" s="5" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D100:E100"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D39:E39"/>
@@ -3918,11 +4824,14 @@
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D125:E125"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3930,75 +4839,121 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7698CA2-98E1-BD48-95D4-F86ECF88AAA6}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="114.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="114.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" t="s">
         <v>295</v>
       </c>
-      <c r="C1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="D2" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="D4" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
keep lib name to avoid test regression
</commit_message>
<xml_diff>
--- a/tools/nist/nist-csf-1.1.xlsx
+++ b/tools/nist/nist-csf-1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EA265D-4B10-3847-99FA-FA26DBB375E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E246623-8FFC-8447-958C-3C39DD4005EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="455">
   <si>
     <t xml:space="preserve">ID.AM-1 </t>
   </si>
@@ -913,9 +913,6 @@
   </si>
   <si>
     <t>library_ref_id</t>
-  </si>
-  <si>
-    <t>NIST CSF version 1.1</t>
   </si>
   <si>
     <t>NIST-CSF-1.1</t>
@@ -1940,9 +1937,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1959,6 +1953,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2318,7 +2315,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2333,7 +2330,7 @@
         <v>270</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2357,7 +2354,7 @@
         <v>288</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2365,7 +2362,7 @@
         <v>273</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2373,7 +2370,7 @@
         <v>274</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2381,7 +2378,7 @@
         <v>286</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2405,15 +2402,15 @@
         <v>276</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2434,7 +2431,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -2442,7 +2439,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -2453,7 +2450,7 @@
         <v>278</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C16" t="s">
         <v>279</v>
@@ -2464,10 +2461,10 @@
         <v>278</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2495,25 +2492,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>295</v>
-      </c>
       <c r="F1" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2526,11 +2523,11 @@
       <c r="D2" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="G2" s="10"/>
+        <v>315</v>
+      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
@@ -2539,18 +2536,18 @@
       <c r="C3" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="G3" s="8"/>
+        <v>316</v>
+      </c>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2562,12 +2559,12 @@
         <v>1</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2579,12 +2576,12 @@
         <v>3</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -2596,12 +2593,12 @@
         <v>5</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -2613,12 +2610,12 @@
         <v>7</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2630,12 +2627,12 @@
         <v>9</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2647,7 +2644,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2657,18 +2654,18 @@
       <c r="C10" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="G10" s="8"/>
+        <v>323</v>
+      </c>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -2680,12 +2677,12 @@
         <v>13</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2697,12 +2694,12 @@
         <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -2714,12 +2711,12 @@
         <v>17</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -2731,12 +2728,12 @@
         <v>19</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -2748,7 +2745,7 @@
         <v>21</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2758,18 +2755,18 @@
       <c r="C16" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="G16" s="8"/>
+        <v>328</v>
+      </c>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -2781,12 +2778,12 @@
         <v>23</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -2798,12 +2795,12 @@
         <v>25</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -2815,12 +2812,12 @@
         <v>27</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2832,7 +2829,7 @@
         <v>29</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2842,18 +2839,18 @@
       <c r="C21" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="G21" s="8"/>
+        <v>333</v>
+      </c>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -2865,12 +2862,12 @@
         <v>31</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -2882,12 +2879,12 @@
         <v>33</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2899,12 +2896,12 @@
         <v>35</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -2916,12 +2913,12 @@
         <v>37</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -2933,12 +2930,12 @@
         <v>39</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -2950,7 +2947,7 @@
         <v>41</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2960,18 +2957,18 @@
       <c r="C28" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="G28" s="8"/>
+        <v>340</v>
+      </c>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -2983,12 +2980,12 @@
         <v>43</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -3000,12 +2997,12 @@
         <v>45</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -3017,7 +3014,7 @@
         <v>47</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3027,18 +3024,18 @@
       <c r="C32" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="13"/>
       <c r="F32" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="G32" s="8"/>
+        <v>344</v>
+      </c>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -3050,12 +3047,12 @@
         <v>49</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -3067,12 +3064,12 @@
         <v>51</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -3084,12 +3081,12 @@
         <v>53</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -3101,12 +3098,12 @@
         <v>55</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -3118,7 +3115,7 @@
         <v>57</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3131,11 +3128,11 @@
       <c r="D38" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E38" s="8"/>
+      <c r="E38" s="7"/>
       <c r="F38" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="G38" s="8"/>
+        <v>350</v>
+      </c>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
@@ -3144,18 +3141,18 @@
       <c r="C39" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="13"/>
       <c r="F39" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="G39" s="8"/>
+        <v>351</v>
+      </c>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -3167,12 +3164,12 @@
         <v>59</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -3184,12 +3181,12 @@
         <v>61</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -3201,12 +3198,12 @@
         <v>63</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -3218,12 +3215,12 @@
         <v>65</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -3235,12 +3232,12 @@
         <v>67</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -3252,12 +3249,12 @@
         <v>69</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -3269,7 +3266,7 @@
         <v>71</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3279,18 +3276,18 @@
       <c r="C47" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="13"/>
       <c r="F47" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="G47" s="8"/>
+        <v>359</v>
+      </c>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -3302,12 +3299,12 @@
         <v>73</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -3319,12 +3316,12 @@
         <v>75</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -3336,12 +3333,12 @@
         <v>77</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -3353,12 +3350,12 @@
         <v>79</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -3370,7 +3367,7 @@
         <v>81</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3380,18 +3377,18 @@
       <c r="C53" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="E53" s="6"/>
+      <c r="E53" s="13"/>
       <c r="F53" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="G53" s="8"/>
+        <v>365</v>
+      </c>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -3403,12 +3400,12 @@
         <v>83</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -3420,12 +3417,12 @@
         <v>85</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -3437,12 +3434,12 @@
         <v>87</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B57">
         <v>3</v>
@@ -3454,12 +3451,12 @@
         <v>89</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -3471,12 +3468,12 @@
         <v>91</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -3488,12 +3485,12 @@
         <v>93</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B60">
         <v>3</v>
@@ -3505,12 +3502,12 @@
         <v>95</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B61">
         <v>3</v>
@@ -3522,7 +3519,7 @@
         <v>97</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3532,18 +3529,18 @@
       <c r="C62" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="E62" s="6"/>
+      <c r="E62" s="13"/>
       <c r="F62" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="G62" s="8"/>
+        <v>374</v>
+      </c>
+      <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B63">
         <v>3</v>
@@ -3555,12 +3552,12 @@
         <v>99</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B64">
         <v>3</v>
@@ -3572,12 +3569,12 @@
         <v>101</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B65">
         <v>3</v>
@@ -3589,12 +3586,12 @@
         <v>103</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -3606,12 +3603,12 @@
         <v>105</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B67">
         <v>3</v>
@@ -3623,12 +3620,12 @@
         <v>107</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B68">
         <v>3</v>
@@ -3640,12 +3637,12 @@
         <v>109</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B69">
         <v>3</v>
@@ -3657,12 +3654,12 @@
         <v>111</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -3674,12 +3671,12 @@
         <v>113</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B71">
         <v>3</v>
@@ -3691,12 +3688,12 @@
         <v>115</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B72">
         <v>3</v>
@@ -3708,12 +3705,12 @@
         <v>117</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B73">
         <v>3</v>
@@ -3725,12 +3722,12 @@
         <v>119</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B74">
         <v>3</v>
@@ -3742,7 +3739,7 @@
         <v>121</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3752,18 +3749,18 @@
       <c r="C75" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="D75" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="E75" s="6"/>
+      <c r="E75" s="13"/>
       <c r="F75" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="G75" s="8"/>
+      <c r="G75" s="7"/>
     </row>
     <row r="76" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B76">
         <v>3</v>
@@ -3775,12 +3772,12 @@
         <v>123</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B77">
         <v>3</v>
@@ -3792,7 +3789,7 @@
         <v>125</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3802,18 +3799,18 @@
       <c r="C78" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D78" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="E78" s="6"/>
+      <c r="E78" s="13"/>
       <c r="F78" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="G78" s="8"/>
+        <v>389</v>
+      </c>
+      <c r="G78" s="7"/>
     </row>
     <row r="79" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B79">
         <v>3</v>
@@ -3825,12 +3822,12 @@
         <v>127</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B80">
         <v>3</v>
@@ -3842,12 +3839,12 @@
         <v>129</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B81">
         <v>3</v>
@@ -3859,12 +3856,12 @@
         <v>131</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B82">
         <v>3</v>
@@ -3876,12 +3873,12 @@
         <v>133</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -3893,7 +3890,7 @@
         <v>135</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3906,11 +3903,11 @@
       <c r="D84" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E84" s="9"/>
+      <c r="E84" s="8"/>
       <c r="F84" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="G84" s="8"/>
+        <v>395</v>
+      </c>
+      <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="2">
@@ -3919,18 +3916,18 @@
       <c r="C85" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="D85" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="E85" s="6"/>
+      <c r="E85" s="13"/>
       <c r="F85" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="G85" s="8"/>
+        <v>396</v>
+      </c>
+      <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B86">
         <v>3</v>
@@ -3942,12 +3939,12 @@
         <v>137</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B87">
         <v>3</v>
@@ -3959,12 +3956,12 @@
         <v>139</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B88">
         <v>3</v>
@@ -3976,12 +3973,12 @@
         <v>141</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B89">
         <v>3</v>
@@ -3993,12 +3990,12 @@
         <v>143</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -4010,7 +4007,7 @@
         <v>145</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4020,18 +4017,18 @@
       <c r="C91" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D91" s="6" t="s">
+      <c r="D91" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E91" s="6"/>
+      <c r="E91" s="13"/>
       <c r="F91" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="G91" s="8"/>
+        <v>402</v>
+      </c>
+      <c r="G91" s="7"/>
     </row>
     <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B92">
         <v>3</v>
@@ -4043,12 +4040,12 @@
         <v>147</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B93">
         <v>3</v>
@@ -4060,12 +4057,12 @@
         <v>149</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B94">
         <v>3</v>
@@ -4077,12 +4074,12 @@
         <v>151</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -4094,12 +4091,12 @@
         <v>153</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B96">
         <v>3</v>
@@ -4111,12 +4108,12 @@
         <v>155</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B97">
         <v>3</v>
@@ -4128,12 +4125,12 @@
         <v>157</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -4145,12 +4142,12 @@
         <v>159</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B99">
         <v>3</v>
@@ -4162,7 +4159,7 @@
         <v>161</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4172,18 +4169,18 @@
       <c r="C100" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="D100" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="E100" s="6"/>
+      <c r="E100" s="13"/>
       <c r="F100" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="G100" s="8"/>
+        <v>411</v>
+      </c>
+      <c r="G100" s="7"/>
     </row>
     <row r="101" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B101">
         <v>3</v>
@@ -4195,12 +4192,12 @@
         <v>163</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -4212,12 +4209,12 @@
         <v>165</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -4229,12 +4226,12 @@
         <v>167</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -4246,12 +4243,12 @@
         <v>169</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -4263,7 +4260,7 @@
         <v>171</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4276,11 +4273,11 @@
       <c r="D106" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E106" s="8"/>
+      <c r="E106" s="7"/>
       <c r="F106" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="G106" s="8"/>
+        <v>417</v>
+      </c>
+      <c r="G106" s="7"/>
     </row>
     <row r="107" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B107" s="2">
@@ -4289,18 +4286,18 @@
       <c r="C107" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D107" s="6" t="s">
+      <c r="D107" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="E107" s="6"/>
+      <c r="E107" s="13"/>
       <c r="F107" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="G107" s="8"/>
+        <v>418</v>
+      </c>
+      <c r="G107" s="7"/>
     </row>
     <row r="108" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -4312,7 +4309,7 @@
         <v>173</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4322,18 +4319,18 @@
       <c r="C109" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D109" s="6" t="s">
+      <c r="D109" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="E109" s="6"/>
+      <c r="E109" s="13"/>
       <c r="F109" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G109" s="8"/>
+      <c r="G109" s="7"/>
     </row>
     <row r="110" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B110">
         <v>3</v>
@@ -4345,12 +4342,12 @@
         <v>175</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -4362,12 +4359,12 @@
         <v>177</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B112">
         <v>3</v>
@@ -4379,12 +4376,12 @@
         <v>179</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B113">
         <v>3</v>
@@ -4396,12 +4393,12 @@
         <v>181</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -4413,7 +4410,7 @@
         <v>183</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4424,18 +4421,18 @@
       <c r="C115" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D115" s="6" t="s">
+      <c r="D115" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="E115" s="6"/>
+      <c r="E115" s="13"/>
       <c r="F115" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="G115" s="8"/>
+        <v>425</v>
+      </c>
+      <c r="G115" s="7"/>
     </row>
     <row r="116" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -4447,12 +4444,12 @@
         <v>185</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -4464,12 +4461,12 @@
         <v>187</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B118">
         <v>3</v>
@@ -4481,12 +4478,12 @@
         <v>189</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B119">
         <v>3</v>
@@ -4498,12 +4495,12 @@
         <v>191</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B120">
         <v>3</v>
@@ -4515,7 +4512,7 @@
         <v>193</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4526,18 +4523,18 @@
       <c r="C121" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D121" s="6" t="s">
+      <c r="D121" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="E121" s="6"/>
+      <c r="E121" s="13"/>
       <c r="F121" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="G121" s="8"/>
+        <v>431</v>
+      </c>
+      <c r="G121" s="7"/>
     </row>
     <row r="122" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B122">
         <v>3</v>
@@ -4549,12 +4546,12 @@
         <v>195</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B123">
         <v>3</v>
@@ -4566,12 +4563,12 @@
         <v>197</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B124">
         <v>3</v>
@@ -4583,7 +4580,7 @@
         <v>199</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4594,18 +4591,18 @@
       <c r="C125" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D125" s="6" t="s">
+      <c r="D125" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="E125" s="6"/>
+      <c r="E125" s="13"/>
       <c r="F125" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="G125" s="8"/>
+        <v>435</v>
+      </c>
+      <c r="G125" s="7"/>
     </row>
     <row r="126" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B126">
         <v>3</v>
@@ -4617,12 +4614,12 @@
         <v>201</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B127">
         <v>3</v>
@@ -4634,7 +4631,7 @@
         <v>203</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4648,11 +4645,11 @@
       <c r="D128" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E128" s="8"/>
+      <c r="E128" s="7"/>
       <c r="F128" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="G128" s="8"/>
+        <v>438</v>
+      </c>
+      <c r="G128" s="7"/>
     </row>
     <row r="129" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129"/>
@@ -4662,18 +4659,18 @@
       <c r="C129" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D129" s="6" t="s">
+      <c r="D129" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="E129" s="6"/>
+      <c r="E129" s="13"/>
       <c r="F129" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="G129" s="8"/>
+        <v>439</v>
+      </c>
+      <c r="G129" s="7"/>
     </row>
     <row r="130" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B130">
         <v>3</v>
@@ -4685,7 +4682,7 @@
         <v>205</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="131" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4696,18 +4693,18 @@
       <c r="C131" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D131" s="6" t="s">
+      <c r="D131" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="E131" s="6"/>
+      <c r="E131" s="13"/>
       <c r="F131" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="G131" s="8"/>
+        <v>435</v>
+      </c>
+      <c r="G131" s="7"/>
     </row>
     <row r="132" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B132">
         <v>3</v>
@@ -4719,12 +4716,12 @@
         <v>207</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B133">
         <v>3</v>
@@ -4736,7 +4733,7 @@
         <v>209</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4747,18 +4744,18 @@
       <c r="C134" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D134" s="6" t="s">
+      <c r="D134" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="E134" s="6"/>
+      <c r="E134" s="13"/>
       <c r="F134" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G134" s="8"/>
+      <c r="G134" s="7"/>
     </row>
     <row r="135" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B135">
         <v>3</v>
@@ -4770,12 +4767,12 @@
         <v>211</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B136">
         <v>3</v>
@@ -4787,12 +4784,12 @@
         <v>213</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B137">
         <v>3</v>
@@ -4804,16 +4801,19 @@
         <v>215</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D125:E125"/>
     <mergeCell ref="D100:E100"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D39:E39"/>
@@ -4824,14 +4824,11 @@
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4855,19 +4852,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" t="s">
         <v>294</v>
       </c>
-      <c r="C1" t="s">
-        <v>295</v>
-      </c>
       <c r="D1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E1" t="s">
         <v>314</v>
-      </c>
-      <c r="E1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -4875,16 +4872,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>452</v>
+      <c r="D2" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -4892,16 +4889,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>451</v>
+      <c r="D3" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -4909,16 +4906,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>449</v>
+      <c r="D4" s="11" t="s">
+        <v>448</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -4926,34 +4923,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>450</v>
+      <c r="D5" s="11" t="s">
+        <v>449</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat(lib): nist csf 1.1 and 2.0 translation in French (#1828)
* translate NIST CSF in FR

* Finish translation in FR

* keep lib name to avoid test regression

* Update sample-domain-schema-1.bak

reflect changes in NIST CSF 2.0

* Update dummy-domain.bak
</commit_message>
<xml_diff>
--- a/tools/nist/nist-csf-1.1.xlsx
+++ b/tools/nist/nist-csf-1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5D501F-78BA-CF4B-A1B0-7347512BA2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E246623-8FFC-8447-958C-3C39DD4005EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="455">
   <si>
     <t xml:space="preserve">ID.AM-1 </t>
   </si>
@@ -915,13 +915,7 @@
     <t>library_ref_id</t>
   </si>
   <si>
-    <t>NIST CSF version 1.1</t>
-  </si>
-  <si>
     <t>NIST-CSF-1.1</t>
-  </si>
-  <si>
-    <t>National Institute of Standards and Technology - Cybersecurity Framework</t>
   </si>
   <si>
     <t>framework_ref_id</t>
@@ -995,13 +989,444 @@
   </si>
   <si>
     <t>scores</t>
+  </si>
+  <si>
+    <t>name[fr]</t>
+  </si>
+  <si>
+    <t>description[fr]</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Gestion des actifs</t>
+  </si>
+  <si>
+    <t>Développez un processus d’inventaire garantissant en permanence un recensement exhaustif de vos équipements TIC (Asset).</t>
+  </si>
+  <si>
+    <t>Inventoriez toutes les plateformes, licences et applications logicielles dans votre entreprise.</t>
+  </si>
+  <si>
+    <t>Listez tous les flux de communication et de transferts de données en interne.</t>
+  </si>
+  <si>
+    <t>Listez tous les systèmes TIC externes cruciaux pour votre entreprise.</t>
+  </si>
+  <si>
+    <t>Etablissez des priorités pour les ressources inventoriées (équipements, données, temps, personnel et applications) selon leur criticité.</t>
+  </si>
+  <si>
+    <t>Définissez clairement les rôles et les responsabilités en matière de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Environnement opérationnel</t>
+  </si>
+  <si>
+    <t>Définissez, documentez et communiquez le rôle exact de votre entreprise dans la chaîne d’approvisionnement (critique).</t>
+  </si>
+  <si>
+    <t>Identifiez et communiquez l’importance de votre entreprise en tant qu’infrastructure vitale et sa position dans le secteur critique.</t>
+  </si>
+  <si>
+    <t>Evaluez et hiérarchisez les objectifs, les tâches et les activités dans l’entreprise.</t>
+  </si>
+  <si>
+    <t>Définissez les exigences de résilience pour les activités de l'entreprise dans toutes les situations opérationnelles (par exemple pendant une prise d'otage ou une attaque, en cas de reprise, en régime nominal).</t>
+  </si>
+  <si>
+    <t>Gouvernance</t>
+  </si>
+  <si>
+    <t>Édictez une politique de sécurité informatique dans votre entreprise.</t>
+  </si>
+  <si>
+    <t>Convenir entre les responsables internes (gestion des risques par ex.) et des partenaires externes, des rôles et des responsabilités en matière de sécurité informatique.</t>
+  </si>
+  <si>
+    <t>Vérifiez que votre entreprise respecte toutes les exigences légales et réglementaires en matière de cybersécurité, y compris au niveau de la protection des données.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les cyber-risques sont bien intégrés dans la gestion des risques pour toute l’entreprise.</t>
+  </si>
+  <si>
+    <t>Évaluation des risques</t>
+  </si>
+  <si>
+    <t>Identifiez les faiblesses (techniques) de vos équipements et documentez-les.</t>
+  </si>
+  <si>
+    <t>Participez à des forums et à des réunions d’experts pour échanger des informations et être au courant des cybermenaces.</t>
+  </si>
+  <si>
+    <t>Identifiez et documentez les cybermenaces, aussi bien internes qu’externes.</t>
+  </si>
+  <si>
+    <t>Identifiez l’impact potentiel des cybermenaces sur vos activités et évaluez leur probabilité d’occurrence.</t>
+  </si>
+  <si>
+    <t>Évaluez les risques pour votre entreprise en fonction des menaces, des vulnérabilités, de l’impact (sur ses activités) et de leur probabilité d’occurrence.</t>
+  </si>
+  <si>
+    <t>Définissez les mesures à prendre immédiatement lorsqu’un risque se concrétise et fixez des priorités.</t>
+  </si>
+  <si>
+    <t>Stratégie de gestion des risques</t>
+  </si>
+  <si>
+    <t>Définissez les processus de gestion des risques, gérez-les activement et faites-les confirmer par les personnes impliquées ou les parties prenantes.</t>
+  </si>
+  <si>
+    <t>Définissez et communiquez les risques supportables pour votre entreprise.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les risques supportables sont évalués en prenant en compte l’importance de votre entreprise du fait qu’elle exploite une infrastructure critique. Prenez également en considération, dans votre analyse, les risques propres au secteur.</t>
+  </si>
+  <si>
+    <t>Gestion des risques liés à la chaine d'approvisionnement</t>
+  </si>
+  <si>
+    <t>Définissez des processus clairs pour gérer les risques liés à une perturbation dans la chaîne d’approvisionnement. Faites contrôler et valider ces processus par toutes les parties prenantes.</t>
+  </si>
+  <si>
+    <t>Identifiez les fournisseurs et les prestataires de services cruciaux pour vos systèmes, composants et services critiques à partir des processus définis ci-dessus et fixez les priorités.</t>
+  </si>
+  <si>
+    <t>Exigez de vos fournisseurs et prestataires de services qu’ils s’engagent contractuellement à développer et mettre en oeuvre des mesures appropriées pour atteindre les objectifs du processus pour gérer les risques liés à la chaîne d’approvisionnement.</t>
+  </si>
+  <si>
+    <t>Faites un suivi systématique pour vous assurer que tous vos fournisseurs et prestataires de services remplissent leurs obligations conformément aux exigences. Faites-le vérifier régulièrement par des rapports d’audit ou par les résultats des tests techniques.</t>
+  </si>
+  <si>
+    <t>Définissez avec vos fournisseurs et prestataires les processus pour réagir et récupérer après des problèmes de cybersécurité. Validez ces processus par des simulations.</t>
+  </si>
+  <si>
+    <t>Protéger</t>
+  </si>
+  <si>
+    <t>Gestion des identités, authentification et contrôle d'accès</t>
+  </si>
+  <si>
+    <t>Définissez un processus clair pour octroyer et gérer les autorisations et les données d’identification pour utilisateurs, appareils/machines et processus.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que seules les personnes autorisées ont physiquement accès aux équipements TIC. Prenez des mesures concrètes pour garantir que les ressources TIC sont protégées contre tout accès physique non autorisé.</t>
+  </si>
+  <si>
+    <t>Définissez les processus pour gérer les accès à distance.</t>
+  </si>
+  <si>
+    <t>Définissez les niveaux d’autorisation en étant le plus restrictif possible et séparez les fonctions.</t>
+  </si>
+  <si>
+    <t>Vérifiez que l’intégrité de votre réseau est protégée. Séparez votre réseau au niveau logique comme physique, si c’est nécessaire et judicieux.</t>
+  </si>
+  <si>
+    <t>N’attribuez des identités numériques qu’à des personnes ou à des processus que vous avez clairement identifiés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les utilisateurs, équipements et autres biens sont authentifés avec un niveau de sécurité (simple facteur, multi-facteur) cohérent avec le risque encouru. </t>
+  </si>
+  <si>
+    <t>Sensibilisation et formation</t>
+  </si>
+  <si>
+    <t>Veillez à ce que tous vos collaborateurs soient sensibilisés et formés en matière de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que les utilisateurs ayant des niveaux d’autorisation élevés soient conscients de leur rôle et de leurs responsabilités.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que tous les acteurs extérieurs à votre entreprise (fournisseurs, clients, partenaires) soient conscients de leur rôle et de leurs responsabilités.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que tous les cadres soient conscients de leurs rôles spécifiques et de leurs responsabilités.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que les responsables de la sécurité physique et de la sécurité informatique soient conscients de leurs rôles spécifiques et de leurs responsabilités.</t>
+  </si>
+  <si>
+    <t>Sécurité des données</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les données stockées sont protégées (contre toute atteinte ou préjudice en termes de confidentialité, d’intégrité et de disponibilité).</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les données sont protégées pendant leur transmission (contre toute atteinte ou préjudice en termes de confidentialité, d’intégrité et de disponibilité).</t>
+  </si>
+  <si>
+    <t>Veillez à ce qu’un processus formel soit défini pour votre matériel TIC afin de protéger les données lorsque des équipements sont supprimés, déplacés ou remplacés.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que vos équipements TIC aient une réserve de capacité suffisante afin que vos données soient toujours disponibles.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que des mesures appropriées sont mises en oeuvre contre les fuites de données.</t>
+  </si>
+  <si>
+    <t>Définissez un processus pour vérifier l’intégrité du micrologiciel, des systèmes d’exploitation, des logiciels d’application et des données.</t>
+  </si>
+  <si>
+    <t>Pour le développement et les tests, ayez un environnement informatique totalement indépendant des systèmes de production.</t>
+  </si>
+  <si>
+    <t>Définissez un processus pour vérifier l’intégrité du matériel utilisé.</t>
+  </si>
+  <si>
+    <t>Processus et procédures de protection de l'information</t>
+  </si>
+  <si>
+    <t>Générez une configuration standard pour l’infrastructure d’information et de communication, ainsi que pour les systèmes de contrôle industriels. Assurez-vous que cette configuration par défaut obéit aux règles usuelles de sécurité (par ex. redondance N-1, configuration minimale, etc.).</t>
+  </si>
+  <si>
+    <t>Définissez un processus « cycle de vie » pour l’utilisation des équipements TIC.</t>
+  </si>
+  <si>
+    <t>Définissez un processus pour contrôler les changements de configuration.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que des sauvegardes informatiques (backups) sont effectuées, gérées et testées régulièrement (+ qu’on peut restaurer les données sauvegardées).</t>
+  </si>
+  <si>
+    <t>Veillez à ce que toutes les exigences (réglementaires) et les directives concernant les équipements « physiques » soient respectées.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que les données soient toujours détruites selon les prescriptions.</t>
+  </si>
+  <si>
+    <t>Développez et améliorez régulièrement vos processus de sécurité informatique.</t>
+  </si>
+  <si>
+    <t>Discutez de l’efficacité des différentes technologies de protection avec vos partenaires.</t>
+  </si>
+  <si>
+    <t>Instaurez des processus pour réagir aux cyberincidents. (Incident Response-Planing, Business Continuity Management, Incident Recovery, Disaster Recovery).</t>
+  </si>
+  <si>
+    <t>Testez les plans de réaction et de récupération.</t>
+  </si>
+  <si>
+    <t>Tenez compte de la cybersécurité dès le processus de recrutement (en vérifiant les antécédents ou par des contrôles de sécurité personnels, par ex.).</t>
+  </si>
+  <si>
+    <t>Développez et mettez en oeuvre un processus pour traiter les failles repérées.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que le fonctionnement, la maintenance et les éventuelles réparations des équipements soient enregistrés et documentés (journalisation). Assurez-vous qu’elles sont effectuées rapidement et en ne recourant qu’à des moyens testés et approuvés.</t>
+  </si>
+  <si>
+    <t>Enregistrez et documentez également les travaux de maintenance de vos systèmes distants. Assurez-vous qu’aucun accès non autorisé n’est possible.</t>
+  </si>
+  <si>
+    <t>Technologie de protection</t>
+  </si>
+  <si>
+    <t>Générez et vérifiez ces fichiers régulièrement, selon les exigences et les directives.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les supports amovibles sont protégés et que leur utilisation se fait dans le strict respect des directives.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que votre système soit configuré pour toujours fonctionner, même en mode dégradé.</t>
+  </si>
+  <si>
+    <t>Assurez la protection de vos réseaux de communication et de contrôle.</t>
+  </si>
+  <si>
+    <t>Définissez des scénarios pour les différents modes de fonctionnement de vos systèmes. Par ex. : fonctionnalités en cas d’attaque, fonctionnalités pendant la phase de récupération, fonctionnalités normales pendant l’exploitation.</t>
+  </si>
+  <si>
+    <t>Détecter</t>
+  </si>
+  <si>
+    <t>Anomalies et événements</t>
+  </si>
+  <si>
+    <t>Définissez des valeurs par défaut pour les opérations réseau licites et les flux de données prévus pour les utilisateurs et les systèmes. Surveillez ces valeurs en permanence.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les incidents de cybersécurité détectés sont analysés quant à leurs objectifs et méthodes.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les informations sur les incidents de cybersécurité provenant de différentes sources et capteurs sont compilées et exploitées.</t>
+  </si>
+  <si>
+    <t>Déterminez les conséquences probables des incidents.</t>
+  </si>
+  <si>
+    <t>Définissez les valeurs limites au-delà desquelles les incidents de cybersécurité doivent générer des alertes.</t>
+  </si>
+  <si>
+    <t>Surveillance continue de la sécurité</t>
+  </si>
+  <si>
+    <t>Mettez en place une surveillance permanente du réseau pour détecter les incidents de cybersécurité potentiels.</t>
+  </si>
+  <si>
+    <t>Mettez en place une surveillance continue (monitorage) de tous les équipements et des bâtiments pour détecter les incidents de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Mettez en place un monitorage de l’utilisation des TIC par les employés pour détecter les incidents de cybersécurité potentiels.</t>
+  </si>
+  <si>
+    <t>Veillez à pouvoir détecter les maliciels.</t>
+  </si>
+  <si>
+    <t>Veillez à pouvoir détecter les maliciels sur les appareils mobiles.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les activités des prestataires de services externes sont surveillées (monitorées) pour détecter d’éventuels incidents de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Surveillez votre système en permanence pour être certain que des activités ou accès liés à des personnes, équipements ou logiciels non autorisés seront détectés.</t>
+  </si>
+  <si>
+    <t>Procédez à des tests de vulnérabilité.</t>
+  </si>
+  <si>
+    <t>Processus de détection</t>
+  </si>
+  <si>
+    <t>Définissez clairement les rôles et les responsabilités pour que tous sachent bien qui est responsable de quoi et qui a telles ou telles compétences.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les processus de détection correspondent aux exigences et conditions fixées.</t>
+  </si>
+  <si>
+    <t>Testez vos processus de détection.</t>
+  </si>
+  <si>
+    <t>Communiquez aux personnes concernées (par ex. fournisseurs, clients, partenaires, autorités) les incidents que vous avez détectés.</t>
+  </si>
+  <si>
+    <t>Améliorez en permanence vos processus de détection.</t>
+  </si>
+  <si>
+    <t>Répondre</t>
+  </si>
+  <si>
+    <t>Planification de la réponse</t>
+  </si>
+  <si>
+    <t>Assurez-vous que le plan d’intervention est correctement suivi et rapidement exécuté si un incident de cybersécurité est détecté.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que toutes les personnes connaissent leurs tâches et la marche à suivre lorsqu’elles doivent réagir à un incident de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Définissez des critères pour les communications et assurez-vous que les incidents de cybersécurité sont signalés et traités conformément à ces critères.</t>
+  </si>
+  <si>
+    <t>Partagez les informations sur les incidents de cybersécurité relevés – ainsi que les enseignements qui en découlent – selon ces critères prédéfinis.</t>
+  </si>
+  <si>
+    <t>Coordonnez-vous avec les parties prenantes selon ces critères.</t>
+  </si>
+  <si>
+    <t>Améliorez la sensibilisation aux incidents de cybersécurité grâce à des échanges réguliers avec vos partenaires.</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les alertes émanant de systèmes de détection sont prises en compte et déclenchent des enquêtes. </t>
+  </si>
+  <si>
+    <t>Veillez à pouvoir évaluer correctement l’impact d’un incident de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Effectuez une analyse technique après chaque incident.</t>
+  </si>
+  <si>
+    <t>Classez les incidents selon les exigences du plan de réaction.</t>
+  </si>
+  <si>
+    <t>Des processus sont établis pour recevoir, analyser et traiter les failles reportées à l'organisation par des sources internes et externes (par exemple lors de tests d'intrusion, via des bulletins de sécurité ou des chercheurs en sécurité).</t>
+  </si>
+  <si>
+    <t>Atténuation</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les incidents de cybersécurité peuvent être circonscrits et que vous pouvez stopper leur propagation.</t>
+  </si>
+  <si>
+    <t>Assurez-vous de pouvoir réduire l’impact des incidents de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Veillez à réduire au maximum les failles récemment découvertes ou référencez-les comme des risques acceptables.</t>
+  </si>
+  <si>
+    <t>Améliorations</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les enseignements tirés des précédents incidents de cybersécurité sont intégrés à vos plans d’intervention.</t>
+  </si>
+  <si>
+    <t>Actualisez vos stratégies de réaction.</t>
+  </si>
+  <si>
+    <t>Rétablir</t>
+  </si>
+  <si>
+    <t>Planification du rétablissement</t>
+  </si>
+  <si>
+    <t>Assurez-vous que le plan de récupération est suivi à la lettre en cas d’incident de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Assurez-vous que les enseignements tirés des précédents incidents de cybersécurité sont intégrés à vos plans de récupération.</t>
+  </si>
+  <si>
+    <t>Actualisez vos stratégies de récupération.</t>
+  </si>
+  <si>
+    <t>Anticipez les réactions du public pour ne pas dégrader la réputation de votre entreprise.</t>
+  </si>
+  <si>
+    <t>Veillez à ce que votre entreprise retrouve vite une image positive après un incident de cybersécurité.</t>
+  </si>
+  <si>
+    <t>Communiquez à l’interne aux parties prenantes tout ce que vous avez entrepris en matière de récupération, sans oublier les cadres et la direction.</t>
+  </si>
+  <si>
+    <t>Partiel</t>
+  </si>
+  <si>
+    <t>Informé des risques</t>
+  </si>
+  <si>
+    <t>Répétable</t>
+  </si>
+  <si>
+    <t>Adaptatif</t>
+  </si>
+  <si>
+    <t>Les pratiques de gestion des risques sont approuvées par la direction, mais ne sont peut-être pas établies comme une politique à l’échelle de l’organisation.
+Il existe une sensibilisation aux risques cybersécurité au niveau de l’organisation, mais une approche globale pour les gérer n’a pas été mise en place.</t>
+  </si>
+  <si>
+    <t>L’application de la stratégie de gestion des risques cybersécurité de l’organisation est gérée de manière ad hoc.
+La sensibilisation aux risques cybersécurité est limitée au niveau organisationnel.
+Les pratiques de gestion des risques sont approuvées par la direction, mais ne sont peut-être pas établies comme une politique à l’échelle de l’organisation.</t>
+  </si>
+  <si>
+    <t>Les pratiques de gestion des risques de l’organisation sont formellement approuvées et exprimées sous forme de politique.
+Les pratiques cybersécurité de l’organisation sont régulièrement mises à jour en fonction de l’application des processus de gestion des risques, pour répondre à l’évolution des exigences métiers ou missions, des menaces et du paysage technologique.</t>
+  </si>
+  <si>
+    <t>L’organisation dispose d’une approche à l’échelle de l’entreprise pour gérer les risques cybersécurité, en utilisant des politiques, processus et procédures informés par les risques pour traiter les événements potentiels.
+L’organisation adapte ses pratiques cybersécurité en fonction des activités passées et présentes, y compris les retours d’expérience et les indicateurs prédictifs.</t>
+  </si>
+  <si>
+    <t>National Institute of Standards and Technology - Cybersecurity Framework (CSF 1.1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1132,6 +1557,21 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1484,7 +1924,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1495,6 +1935,23 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1858,7 +2315,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1873,7 +2330,7 @@
         <v>270</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1881,7 +2338,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1897,7 +2354,7 @@
         <v>288</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1905,7 +2362,7 @@
         <v>273</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1913,7 +2370,7 @@
         <v>274</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>291</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1921,7 +2378,7 @@
         <v>286</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1945,15 +2402,15 @@
         <v>276</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1974,7 +2431,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -1982,7 +2439,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -1993,7 +2450,7 @@
         <v>278</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C16" t="s">
         <v>279</v>
@@ -2004,10 +2461,10 @@
         <v>278</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C17" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2017,37 +2474,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="186.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="61.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="103.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -2057,22 +2523,31 @@
       <c r="D2" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="7"/>
+      <c r="F2" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="13"/>
+      <c r="F3" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2080,13 +2555,16 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2094,13 +2572,16 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -2108,13 +2589,16 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -2122,13 +2606,16 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2136,13 +2623,16 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2150,25 +2640,32 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G9" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="13"/>
+      <c r="F10" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -2176,13 +2673,16 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G11" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2190,13 +2690,16 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G12" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -2204,13 +2707,16 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -2218,13 +2724,16 @@
       <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G14" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -2232,25 +2741,32 @@
       <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="13"/>
+      <c r="F16" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -2258,13 +2774,16 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G17" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -2272,13 +2791,16 @@
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G18" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -2286,13 +2808,16 @@
       <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G19" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2300,25 +2825,32 @@
       <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G20" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="13"/>
+      <c r="F21" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -2326,13 +2858,16 @@
       <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G22" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -2340,13 +2875,16 @@
       <c r="C23" t="s">
         <v>32</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G23" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2354,13 +2892,16 @@
       <c r="C24" t="s">
         <v>34</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G24" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -2368,13 +2909,16 @@
       <c r="C25" t="s">
         <v>36</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G25" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -2382,13 +2926,16 @@
       <c r="C26" t="s">
         <v>38</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G26" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -2396,25 +2943,32 @@
       <c r="C27" t="s">
         <v>40</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="13"/>
+      <c r="F28" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -2422,13 +2976,16 @@
       <c r="C29" t="s">
         <v>42</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G29" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -2436,13 +2993,16 @@
       <c r="C30" t="s">
         <v>44</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G30" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -2450,25 +3010,32 @@
       <c r="C31" t="s">
         <v>46</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G31" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="13"/>
+      <c r="F32" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -2476,13 +3043,16 @@
       <c r="C33" t="s">
         <v>48</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G33" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -2490,13 +3060,16 @@
       <c r="C34" t="s">
         <v>50</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G34" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -2504,13 +3077,16 @@
       <c r="C35" t="s">
         <v>52</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G35" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -2518,13 +3094,16 @@
       <c r="C36" t="s">
         <v>54</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G36" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -2532,11 +3111,14 @@
       <c r="C37" t="s">
         <v>56</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G37" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
         <v>1</v>
       </c>
@@ -2546,22 +3128,31 @@
       <c r="D38" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E38" s="7"/>
+      <c r="F38" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="13"/>
+      <c r="F39" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -2569,13 +3160,16 @@
       <c r="C40" t="s">
         <v>58</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G40" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -2583,13 +3177,16 @@
       <c r="C41" t="s">
         <v>60</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G41" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -2597,13 +3194,16 @@
       <c r="C42" t="s">
         <v>62</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G42" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -2611,13 +3211,16 @@
       <c r="C43" t="s">
         <v>64</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G43" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -2625,13 +3228,16 @@
       <c r="C44" t="s">
         <v>66</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G44" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -2639,13 +3245,16 @@
       <c r="C45" t="s">
         <v>68</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G45" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -2653,25 +3262,32 @@
       <c r="C46" t="s">
         <v>70</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G46" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" s="2">
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E47" s="13"/>
+      <c r="F47" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -2679,13 +3295,16 @@
       <c r="C48" t="s">
         <v>72</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G48" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -2693,13 +3312,16 @@
       <c r="C49" t="s">
         <v>74</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G49" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -2707,13 +3329,16 @@
       <c r="C50" t="s">
         <v>76</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G50" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -2721,13 +3346,16 @@
       <c r="C51" t="s">
         <v>78</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G51" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -2735,25 +3363,32 @@
       <c r="C52" t="s">
         <v>80</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G52" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="2">
         <v>2</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E53" s="13"/>
+      <c r="F53" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -2761,13 +3396,16 @@
       <c r="C54" t="s">
         <v>82</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G54" s="5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -2775,13 +3413,16 @@
       <c r="C55" t="s">
         <v>84</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G55" s="5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -2789,13 +3430,16 @@
       <c r="C56" t="s">
         <v>86</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G56" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B57">
         <v>3</v>
@@ -2803,13 +3447,16 @@
       <c r="C57" t="s">
         <v>88</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G57" s="5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -2817,13 +3464,16 @@
       <c r="C58" t="s">
         <v>90</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G58" s="5" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -2831,13 +3481,16 @@
       <c r="C59" t="s">
         <v>92</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G59" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B60">
         <v>3</v>
@@ -2845,13 +3498,16 @@
       <c r="C60" t="s">
         <v>94</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G60" s="5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B61">
         <v>3</v>
@@ -2859,25 +3515,32 @@
       <c r="C61" t="s">
         <v>96</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G61" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2">
         <v>2</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E62" s="13"/>
+      <c r="F62" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B63">
         <v>3</v>
@@ -2885,13 +3548,16 @@
       <c r="C63" t="s">
         <v>98</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G63" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B64">
         <v>3</v>
@@ -2899,13 +3565,16 @@
       <c r="C64" t="s">
         <v>100</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G64" s="5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B65">
         <v>3</v>
@@ -2913,13 +3582,16 @@
       <c r="C65" t="s">
         <v>102</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G65" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -2927,13 +3599,16 @@
       <c r="C66" t="s">
         <v>104</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G66" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B67">
         <v>3</v>
@@ -2941,13 +3616,16 @@
       <c r="C67" t="s">
         <v>106</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G67" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B68">
         <v>3</v>
@@ -2955,13 +3633,16 @@
       <c r="C68" t="s">
         <v>108</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G68" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B69">
         <v>3</v>
@@ -2969,13 +3650,16 @@
       <c r="C69" t="s">
         <v>110</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G69" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -2983,13 +3667,16 @@
       <c r="C70" t="s">
         <v>112</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G70" s="5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B71">
         <v>3</v>
@@ -2997,13 +3684,16 @@
       <c r="C71" t="s">
         <v>114</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G71" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B72">
         <v>3</v>
@@ -3011,13 +3701,16 @@
       <c r="C72" t="s">
         <v>116</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G72" s="5" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B73">
         <v>3</v>
@@ -3025,13 +3718,16 @@
       <c r="C73" t="s">
         <v>118</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G73" s="5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B74">
         <v>3</v>
@@ -3039,25 +3735,32 @@
       <c r="C74" t="s">
         <v>120</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G74" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="2">
         <v>2</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="D75" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="E75" s="6"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E75" s="13"/>
+      <c r="F75" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B76">
         <v>3</v>
@@ -3065,13 +3768,16 @@
       <c r="C76" t="s">
         <v>122</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G76" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B77">
         <v>3</v>
@@ -3079,25 +3785,32 @@
       <c r="C77" t="s">
         <v>124</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G77" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="2">
         <v>2</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D78" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E78" s="13"/>
+      <c r="F78" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G78" s="7"/>
+    </row>
+    <row r="79" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B79">
         <v>3</v>
@@ -3105,13 +3818,16 @@
       <c r="C79" t="s">
         <v>126</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G79" s="5" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B80">
         <v>3</v>
@@ -3119,13 +3835,16 @@
       <c r="C80" t="s">
         <v>128</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G80" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B81">
         <v>3</v>
@@ -3133,13 +3852,16 @@
       <c r="C81" t="s">
         <v>130</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G81" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B82">
         <v>3</v>
@@ -3147,13 +3869,16 @@
       <c r="C82" t="s">
         <v>132</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="5" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G82" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -3161,11 +3886,14 @@
       <c r="C83" t="s">
         <v>134</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G83" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B84" s="2">
         <v>1</v>
       </c>
@@ -3175,23 +3903,31 @@
       <c r="D84" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E84" s="8"/>
+      <c r="F84" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="G84" s="7"/>
+    </row>
+    <row r="85" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="2">
         <v>2</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="D85" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="E85" s="6"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E85" s="13"/>
+      <c r="F85" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G85" s="7"/>
+    </row>
+    <row r="86" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B86">
         <v>3</v>
@@ -3199,13 +3935,16 @@
       <c r="C86" t="s">
         <v>136</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G86" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B87">
         <v>3</v>
@@ -3213,13 +3952,16 @@
       <c r="C87" t="s">
         <v>138</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G87" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B88">
         <v>3</v>
@@ -3227,13 +3969,16 @@
       <c r="C88" t="s">
         <v>140</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G88" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B89">
         <v>3</v>
@@ -3241,13 +3986,16 @@
       <c r="C89" t="s">
         <v>142</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G89" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -3255,25 +4003,32 @@
       <c r="C90" t="s">
         <v>144</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G90" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B91" s="2">
         <v>2</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D91" s="6" t="s">
+      <c r="D91" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E91" s="6"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E91" s="13"/>
+      <c r="F91" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="G91" s="7"/>
+    </row>
+    <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B92">
         <v>3</v>
@@ -3281,13 +4036,16 @@
       <c r="C92" t="s">
         <v>146</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G92" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B93">
         <v>3</v>
@@ -3295,13 +4053,16 @@
       <c r="C93" t="s">
         <v>148</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G93" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B94">
         <v>3</v>
@@ -3309,13 +4070,16 @@
       <c r="C94" t="s">
         <v>150</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="5" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G94" s="5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -3323,13 +4087,16 @@
       <c r="C95" t="s">
         <v>152</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="5" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G95" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B96">
         <v>3</v>
@@ -3337,13 +4104,16 @@
       <c r="C96" t="s">
         <v>154</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G96" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B97">
         <v>3</v>
@@ -3351,13 +4121,16 @@
       <c r="C97" t="s">
         <v>156</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="5" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G97" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -3365,13 +4138,16 @@
       <c r="C98" t="s">
         <v>158</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="5" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G98" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B99">
         <v>3</v>
@@ -3379,25 +4155,32 @@
       <c r="C99" t="s">
         <v>160</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="5" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G99" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B100" s="2">
         <v>2</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="D100" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="E100" s="6"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E100" s="13"/>
+      <c r="F100" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G100" s="7"/>
+    </row>
+    <row r="101" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B101">
         <v>3</v>
@@ -3405,13 +4188,16 @@
       <c r="C101" t="s">
         <v>162</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="5" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G101" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -3419,13 +4205,16 @@
       <c r="C102" t="s">
         <v>164</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G102" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -3433,13 +4222,16 @@
       <c r="C103" t="s">
         <v>166</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E103" s="5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G103" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -3447,13 +4239,16 @@
       <c r="C104" t="s">
         <v>168</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="5" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G104" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -3461,11 +4256,14 @@
       <c r="C105" t="s">
         <v>170</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="5" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G105" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B106" s="2">
         <v>1</v>
       </c>
@@ -3475,22 +4273,31 @@
       <c r="D106" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E106" s="7"/>
+      <c r="F106" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="G106" s="7"/>
+    </row>
+    <row r="107" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B107" s="2">
         <v>2</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D107" s="6" t="s">
+      <c r="D107" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="E107" s="6"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E107" s="13"/>
+      <c r="F107" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="G107" s="7"/>
+    </row>
+    <row r="108" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -3498,25 +4305,32 @@
       <c r="C108" t="s">
         <v>172</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="5" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G108" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B109" s="2">
         <v>2</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D109" s="6" t="s">
+      <c r="D109" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="E109" s="6"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E109" s="13"/>
+      <c r="F109" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G109" s="7"/>
+    </row>
+    <row r="110" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B110">
         <v>3</v>
@@ -3524,13 +4338,16 @@
       <c r="C110" t="s">
         <v>174</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="5" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G110" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -3538,13 +4355,16 @@
       <c r="C111" t="s">
         <v>176</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="5" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G111" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B112">
         <v>3</v>
@@ -3552,13 +4372,16 @@
       <c r="C112" t="s">
         <v>178</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="5" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G112" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B113">
         <v>3</v>
@@ -3566,13 +4389,16 @@
       <c r="C113" t="s">
         <v>180</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="5" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G113" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -3580,11 +4406,14 @@
       <c r="C114" t="s">
         <v>182</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="5" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G114" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115"/>
       <c r="B115" s="2">
         <v>2</v>
@@ -3592,14 +4421,18 @@
       <c r="C115" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D115" s="6" t="s">
+      <c r="D115" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="E115" s="6"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E115" s="13"/>
+      <c r="F115" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="G115" s="7"/>
+    </row>
+    <row r="116" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -3607,13 +4440,16 @@
       <c r="C116" t="s">
         <v>184</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="5" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G116" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -3621,13 +4457,16 @@
       <c r="C117" t="s">
         <v>186</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="5" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G117" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B118">
         <v>3</v>
@@ -3635,13 +4474,16 @@
       <c r="C118" t="s">
         <v>188</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="5" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G118" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B119">
         <v>3</v>
@@ -3649,13 +4491,16 @@
       <c r="C119" t="s">
         <v>190</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E119" s="5" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G119" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B120">
         <v>3</v>
@@ -3663,11 +4508,14 @@
       <c r="C120" t="s">
         <v>192</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="5" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G120" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121"/>
       <c r="B121" s="2">
         <v>2</v>
@@ -3675,14 +4523,18 @@
       <c r="C121" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D121" s="6" t="s">
+      <c r="D121" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="E121" s="6"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E121" s="13"/>
+      <c r="F121" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="G121" s="7"/>
+    </row>
+    <row r="122" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B122">
         <v>3</v>
@@ -3690,13 +4542,16 @@
       <c r="C122" t="s">
         <v>194</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="5" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G122" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B123">
         <v>3</v>
@@ -3704,13 +4559,16 @@
       <c r="C123" t="s">
         <v>196</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="5" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G123" s="5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B124">
         <v>3</v>
@@ -3718,11 +4576,14 @@
       <c r="C124" t="s">
         <v>198</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="5" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G124" s="5" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125"/>
       <c r="B125" s="2">
         <v>2</v>
@@ -3730,14 +4591,18 @@
       <c r="C125" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D125" s="6" t="s">
+      <c r="D125" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="E125" s="6"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E125" s="13"/>
+      <c r="F125" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G125" s="7"/>
+    </row>
+    <row r="126" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B126">
         <v>3</v>
@@ -3745,13 +4610,16 @@
       <c r="C126" t="s">
         <v>200</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="5" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G126" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B127">
         <v>3</v>
@@ -3759,11 +4627,14 @@
       <c r="C127" t="s">
         <v>202</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="5" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G127" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128"/>
       <c r="B128" s="2">
         <v>1</v>
@@ -3774,8 +4645,13 @@
       <c r="D128" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E128" s="7"/>
+      <c r="F128" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="G128" s="7"/>
+    </row>
+    <row r="129" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129"/>
       <c r="B129" s="2">
         <v>2</v>
@@ -3783,14 +4659,18 @@
       <c r="C129" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D129" s="6" t="s">
+      <c r="D129" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="E129" s="6"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E129" s="13"/>
+      <c r="F129" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="G129" s="7"/>
+    </row>
+    <row r="130" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B130">
         <v>3</v>
@@ -3798,11 +4678,14 @@
       <c r="C130" t="s">
         <v>204</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="5" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G130" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131"/>
       <c r="B131" s="2">
         <v>2</v>
@@ -3810,14 +4693,18 @@
       <c r="C131" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D131" s="6" t="s">
+      <c r="D131" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="E131" s="6"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E131" s="13"/>
+      <c r="F131" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G131" s="7"/>
+    </row>
+    <row r="132" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B132">
         <v>3</v>
@@ -3825,13 +4712,16 @@
       <c r="C132" t="s">
         <v>206</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E132" s="5" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G132" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B133">
         <v>3</v>
@@ -3839,11 +4729,14 @@
       <c r="C133" t="s">
         <v>208</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G133" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134"/>
       <c r="B134" s="2">
         <v>2</v>
@@ -3851,14 +4744,18 @@
       <c r="C134" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D134" s="6" t="s">
+      <c r="D134" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="E134" s="6"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E134" s="13"/>
+      <c r="F134" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G134" s="7"/>
+    </row>
+    <row r="135" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B135">
         <v>3</v>
@@ -3866,13 +4763,16 @@
       <c r="C135" t="s">
         <v>210</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E135" s="5" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G135" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B136">
         <v>3</v>
@@ -3880,13 +4780,16 @@
       <c r="C136" t="s">
         <v>212</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E136" s="5" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G136" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B137">
         <v>3</v>
@@ -3894,8 +4797,11 @@
       <c r="C137" t="s">
         <v>214</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E137" s="5" t="s">
         <v>215</v>
+      </c>
+      <c r="G137" s="5" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -3930,75 +4836,121 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7698CA2-98E1-BD48-95D4-F86ECF88AAA6}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="114.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="114.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+      <c r="D1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>306</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="D4" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
show FR language availability for nist csf 1.1
</commit_message>
<xml_diff>
--- a/tools/nist/nist-csf-1.1.xlsx
+++ b/tools/nist/nist-csf-1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E246623-8FFC-8447-958C-3C39DD4005EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22D3A3-0A74-BA47-807F-F28F5B900A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="458">
   <si>
     <t xml:space="preserve">ID.AM-1 </t>
   </si>
@@ -1420,13 +1420,22 @@
   </si>
   <si>
     <t>National Institute of Standards and Technology - Cybersecurity Framework (CSF 1.1)</t>
+  </si>
+  <si>
+    <t>library_name[fr]</t>
+  </si>
+  <si>
+    <t>library_description[fr]</t>
+  </si>
+  <si>
+    <t>NIST CSF version 1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1572,6 +1581,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1924,7 +1940,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1957,6 +1973,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2312,10 +2329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B396070-5818-EE4E-B35D-33D5A66914F0}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2338,7 +2355,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2465,6 +2482,22 @@
       </c>
       <c r="C17" t="s">
         <v>312</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>455</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4806,14 +4839,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D100:E100"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D39:E39"/>
@@ -4824,11 +4854,14 @@
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D125:E125"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix(lib): show FR language availability for nist csf 1.1 (#1907)
show FR language availability for nist csf 1.1
</commit_message>
<xml_diff>
--- a/tools/nist/nist-csf-1.1.xlsx
+++ b/tools/nist/nist-csf-1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E246623-8FFC-8447-958C-3C39DD4005EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22D3A3-0A74-BA47-807F-F28F5B900A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="458">
   <si>
     <t xml:space="preserve">ID.AM-1 </t>
   </si>
@@ -1420,13 +1420,22 @@
   </si>
   <si>
     <t>National Institute of Standards and Technology - Cybersecurity Framework (CSF 1.1)</t>
+  </si>
+  <si>
+    <t>library_name[fr]</t>
+  </si>
+  <si>
+    <t>library_description[fr]</t>
+  </si>
+  <si>
+    <t>NIST CSF version 1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1572,6 +1581,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1924,7 +1940,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1957,6 +1973,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2312,10 +2329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B396070-5818-EE4E-B35D-33D5A66914F0}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2338,7 +2355,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2465,6 +2482,22 @@
       </c>
       <c r="C17" t="s">
         <v>312</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>455</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4806,14 +4839,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D100:E100"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D39:E39"/>
@@ -4824,11 +4854,14 @@
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D125:E125"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix nist-csf 1.1 translations
</commit_message>
<xml_diff>
--- a/tools/nist/nist-csf-1.1.xlsx
+++ b/tools/nist/nist-csf-1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22D3A3-0A74-BA47-807F-F28F5B900A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755B1237-F187-884F-826F-0CE8F404FBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="459">
   <si>
     <t xml:space="preserve">ID.AM-1 </t>
   </si>
@@ -1010,9 +1010,6 @@
   </si>
   <si>
     <t>Listez tous les flux de communication et de transferts de données en interne.</t>
-  </si>
-  <si>
-    <t>Listez tous les systèmes TIC externes cruciaux pour votre entreprise.</t>
   </si>
   <si>
     <t>Etablissez des priorités pour les ressources inventoriées (équipements, données, temps, personnel et applications) selon leur criticité.</t>
@@ -1429,6 +1426,12 @@
   </si>
   <si>
     <t>NIST CSF version 1.1</t>
+  </si>
+  <si>
+    <t>Identifiez et formalisez les dépendances et les fonctions critiques nécessaires à la fourniture des services essentiels.</t>
+  </si>
+  <si>
+    <t>Listez tous les systèmes TIC externes.</t>
   </si>
 </sst>
 </file>
@@ -1970,10 +1973,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2331,7 +2334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B396070-5818-EE4E-B35D-33D5A66914F0}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2355,7 +2358,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2387,7 +2390,7 @@
         <v>274</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2485,19 +2488,19 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>456</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>454</v>
+      <c r="B19" s="13" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -2509,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2569,10 +2572,10 @@
       <c r="C3" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="2" t="s">
         <v>316</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>320</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2660,7 +2663,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2677,7 +2680,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2687,12 +2690,12 @@
       <c r="C10" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G10" s="7"/>
     </row>
@@ -2710,7 +2713,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2727,7 +2730,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2744,7 +2747,7 @@
         <v>17</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2761,7 +2764,7 @@
         <v>19</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>320</v>
+        <v>457</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2778,7 +2781,7 @@
         <v>21</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2788,12 +2791,12 @@
       <c r="C16" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G16" s="7"/>
     </row>
@@ -2811,7 +2814,7 @@
         <v>23</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2828,7 +2831,7 @@
         <v>25</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2845,7 +2848,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2862,7 +2865,7 @@
         <v>29</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2872,12 +2875,12 @@
       <c r="C21" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G21" s="7"/>
     </row>
@@ -2895,7 +2898,7 @@
         <v>31</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2912,7 +2915,7 @@
         <v>33</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2929,7 +2932,7 @@
         <v>35</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2946,7 +2949,7 @@
         <v>37</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2963,7 +2966,7 @@
         <v>39</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2980,7 +2983,7 @@
         <v>41</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2990,12 +2993,12 @@
       <c r="C28" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G28" s="7"/>
     </row>
@@ -3013,7 +3016,7 @@
         <v>43</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3030,7 +3033,7 @@
         <v>45</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3047,7 +3050,7 @@
         <v>47</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3057,12 +3060,12 @@
       <c r="C32" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="E32" s="13"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G32" s="7"/>
     </row>
@@ -3080,7 +3083,7 @@
         <v>49</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3097,7 +3100,7 @@
         <v>51</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -3114,7 +3117,7 @@
         <v>53</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3131,7 +3134,7 @@
         <v>55</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3148,7 +3151,7 @@
         <v>57</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3163,7 +3166,7 @@
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G38" s="7"/>
     </row>
@@ -3174,12 +3177,12 @@
       <c r="C39" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="E39" s="13"/>
+      <c r="E39" s="14"/>
       <c r="F39" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G39" s="7"/>
     </row>
@@ -3197,7 +3200,7 @@
         <v>59</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3214,7 +3217,7 @@
         <v>61</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3231,7 +3234,7 @@
         <v>63</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3248,7 +3251,7 @@
         <v>65</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3265,7 +3268,7 @@
         <v>67</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3282,7 +3285,7 @@
         <v>69</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3299,7 +3302,7 @@
         <v>71</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3309,12 +3312,12 @@
       <c r="C47" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="E47" s="13"/>
+      <c r="E47" s="14"/>
       <c r="F47" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G47" s="7"/>
     </row>
@@ -3332,7 +3335,7 @@
         <v>73</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3349,7 +3352,7 @@
         <v>75</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3366,7 +3369,7 @@
         <v>77</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3383,7 +3386,7 @@
         <v>79</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3400,7 +3403,7 @@
         <v>81</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3410,12 +3413,12 @@
       <c r="C53" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="E53" s="13"/>
+      <c r="E53" s="14"/>
       <c r="F53" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G53" s="7"/>
     </row>
@@ -3433,7 +3436,7 @@
         <v>83</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3450,7 +3453,7 @@
         <v>85</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3467,7 +3470,7 @@
         <v>87</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3484,7 +3487,7 @@
         <v>89</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3501,7 +3504,7 @@
         <v>91</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3518,7 +3521,7 @@
         <v>93</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3535,7 +3538,7 @@
         <v>95</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3552,7 +3555,7 @@
         <v>97</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3562,12 +3565,12 @@
       <c r="C62" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="E62" s="13"/>
+      <c r="E62" s="14"/>
       <c r="F62" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G62" s="7"/>
     </row>
@@ -3585,7 +3588,7 @@
         <v>99</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3602,7 +3605,7 @@
         <v>101</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3619,7 +3622,7 @@
         <v>103</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3636,7 +3639,7 @@
         <v>105</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3653,7 +3656,7 @@
         <v>107</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3670,7 +3673,7 @@
         <v>109</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3687,7 +3690,7 @@
         <v>111</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3704,7 +3707,7 @@
         <v>113</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3721,7 +3724,7 @@
         <v>115</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3738,7 +3741,7 @@
         <v>117</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3755,7 +3758,7 @@
         <v>119</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3772,7 +3775,7 @@
         <v>121</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3782,10 +3785,10 @@
       <c r="C75" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D75" s="13" t="s">
+      <c r="D75" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="E75" s="13"/>
+      <c r="E75" s="14"/>
       <c r="F75" s="2" t="s">
         <v>244</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>123</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3822,7 +3825,7 @@
         <v>125</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3832,12 +3835,12 @@
       <c r="C78" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D78" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="E78" s="13"/>
+      <c r="E78" s="14"/>
       <c r="F78" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G78" s="7"/>
     </row>
@@ -3855,7 +3858,7 @@
         <v>127</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3872,7 +3875,7 @@
         <v>129</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3889,7 +3892,7 @@
         <v>131</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3906,7 +3909,7 @@
         <v>133</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3923,7 +3926,7 @@
         <v>135</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3938,7 +3941,7 @@
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G84" s="7"/>
     </row>
@@ -3949,12 +3952,12 @@
       <c r="C85" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D85" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="E85" s="13"/>
+      <c r="E85" s="14"/>
       <c r="F85" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G85" s="7"/>
     </row>
@@ -3972,7 +3975,7 @@
         <v>137</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3989,7 +3992,7 @@
         <v>139</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4006,7 +4009,7 @@
         <v>141</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4023,7 +4026,7 @@
         <v>143</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4040,7 +4043,7 @@
         <v>145</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4050,12 +4053,12 @@
       <c r="C91" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D91" s="13" t="s">
+      <c r="D91" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E91" s="13"/>
+      <c r="E91" s="14"/>
       <c r="F91" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G91" s="7"/>
     </row>
@@ -4073,7 +4076,7 @@
         <v>147</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4090,7 +4093,7 @@
         <v>149</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4107,7 +4110,7 @@
         <v>151</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4124,7 +4127,7 @@
         <v>153</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4141,7 +4144,7 @@
         <v>155</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4158,7 +4161,7 @@
         <v>157</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4175,7 +4178,7 @@
         <v>159</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4192,7 +4195,7 @@
         <v>161</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4202,12 +4205,12 @@
       <c r="C100" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D100" s="13" t="s">
+      <c r="D100" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="E100" s="13"/>
+      <c r="E100" s="14"/>
       <c r="F100" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G100" s="7"/>
     </row>
@@ -4225,7 +4228,7 @@
         <v>163</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4242,7 +4245,7 @@
         <v>165</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4259,7 +4262,7 @@
         <v>167</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4276,7 +4279,7 @@
         <v>169</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4293,7 +4296,7 @@
         <v>171</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4308,7 +4311,7 @@
       </c>
       <c r="E106" s="7"/>
       <c r="F106" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G106" s="7"/>
     </row>
@@ -4319,12 +4322,12 @@
       <c r="C107" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D107" s="13" t="s">
+      <c r="D107" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="E107" s="13"/>
+      <c r="E107" s="14"/>
       <c r="F107" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G107" s="7"/>
     </row>
@@ -4342,7 +4345,7 @@
         <v>173</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4352,10 +4355,10 @@
       <c r="C109" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D109" s="13" t="s">
+      <c r="D109" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="E109" s="13"/>
+      <c r="E109" s="14"/>
       <c r="F109" s="2" t="s">
         <v>266</v>
       </c>
@@ -4375,7 +4378,7 @@
         <v>175</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4392,7 +4395,7 @@
         <v>177</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4409,7 +4412,7 @@
         <v>179</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4426,7 +4429,7 @@
         <v>181</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4443,7 +4446,7 @@
         <v>183</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4454,12 +4457,12 @@
       <c r="C115" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D115" s="13" t="s">
+      <c r="D115" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="E115" s="13"/>
+      <c r="E115" s="14"/>
       <c r="F115" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G115" s="7"/>
     </row>
@@ -4477,7 +4480,7 @@
         <v>185</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4494,7 +4497,7 @@
         <v>187</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4511,7 +4514,7 @@
         <v>189</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4528,7 +4531,7 @@
         <v>191</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -4545,7 +4548,7 @@
         <v>193</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4556,12 +4559,12 @@
       <c r="C121" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D121" s="13" t="s">
+      <c r="D121" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="E121" s="13"/>
+      <c r="E121" s="14"/>
       <c r="F121" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G121" s="7"/>
     </row>
@@ -4579,7 +4582,7 @@
         <v>195</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4596,7 +4599,7 @@
         <v>197</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4613,7 +4616,7 @@
         <v>199</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4624,12 +4627,12 @@
       <c r="C125" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D125" s="13" t="s">
+      <c r="D125" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="E125" s="13"/>
+      <c r="E125" s="14"/>
       <c r="F125" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G125" s="7"/>
     </row>
@@ -4647,7 +4650,7 @@
         <v>201</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4664,7 +4667,7 @@
         <v>203</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4680,7 +4683,7 @@
       </c>
       <c r="E128" s="7"/>
       <c r="F128" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G128" s="7"/>
     </row>
@@ -4692,12 +4695,12 @@
       <c r="C129" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D129" s="13" t="s">
+      <c r="D129" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="E129" s="13"/>
+      <c r="E129" s="14"/>
       <c r="F129" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G129" s="7"/>
     </row>
@@ -4715,7 +4718,7 @@
         <v>205</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="131" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4726,12 +4729,12 @@
       <c r="C131" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D131" s="13" t="s">
+      <c r="D131" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="E131" s="13"/>
+      <c r="E131" s="14"/>
       <c r="F131" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G131" s="7"/>
     </row>
@@ -4749,7 +4752,7 @@
         <v>207</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4766,7 +4769,7 @@
         <v>209</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4777,10 +4780,10 @@
       <c r="C134" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D134" s="13" t="s">
+      <c r="D134" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="E134" s="13"/>
+      <c r="E134" s="14"/>
       <c r="F134" s="2" t="s">
         <v>266</v>
       </c>
@@ -4800,7 +4803,7 @@
         <v>211</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4817,7 +4820,7 @@
         <v>213</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4834,16 +4837,19 @@
         <v>215</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D125:E125"/>
     <mergeCell ref="D100:E100"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D39:E39"/>
@@ -4854,14 +4860,11 @@
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4911,10 +4914,10 @@
         <v>303</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -4928,10 +4931,10 @@
         <v>305</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -4945,10 +4948,10 @@
         <v>307</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -4962,10 +4965,10 @@
         <v>309</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix(lib): fix nist-csf 1.1 translations (#2017)
fix nist-csf 1.1 translations
</commit_message>
<xml_diff>
--- a/tools/nist/nist-csf-1.1.xlsx
+++ b/tools/nist/nist-csf-1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22D3A3-0A74-BA47-807F-F28F5B900A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755B1237-F187-884F-826F-0CE8F404FBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="459">
   <si>
     <t xml:space="preserve">ID.AM-1 </t>
   </si>
@@ -1010,9 +1010,6 @@
   </si>
   <si>
     <t>Listez tous les flux de communication et de transferts de données en interne.</t>
-  </si>
-  <si>
-    <t>Listez tous les systèmes TIC externes cruciaux pour votre entreprise.</t>
   </si>
   <si>
     <t>Etablissez des priorités pour les ressources inventoriées (équipements, données, temps, personnel et applications) selon leur criticité.</t>
@@ -1429,6 +1426,12 @@
   </si>
   <si>
     <t>NIST CSF version 1.1</t>
+  </si>
+  <si>
+    <t>Identifiez et formalisez les dépendances et les fonctions critiques nécessaires à la fourniture des services essentiels.</t>
+  </si>
+  <si>
+    <t>Listez tous les systèmes TIC externes.</t>
   </si>
 </sst>
 </file>
@@ -1970,10 +1973,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2331,7 +2334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B396070-5818-EE4E-B35D-33D5A66914F0}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2355,7 +2358,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2387,7 +2390,7 @@
         <v>274</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2485,19 +2488,19 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>456</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>454</v>
+      <c r="B19" s="13" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -2509,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2569,10 +2572,10 @@
       <c r="C3" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="2" t="s">
         <v>316</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>320</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2660,7 +2663,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2677,7 +2680,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2687,12 +2690,12 @@
       <c r="C10" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G10" s="7"/>
     </row>
@@ -2710,7 +2713,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2727,7 +2730,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2744,7 +2747,7 @@
         <v>17</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2761,7 +2764,7 @@
         <v>19</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>320</v>
+        <v>457</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2778,7 +2781,7 @@
         <v>21</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2788,12 +2791,12 @@
       <c r="C16" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G16" s="7"/>
     </row>
@@ -2811,7 +2814,7 @@
         <v>23</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2828,7 +2831,7 @@
         <v>25</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2845,7 +2848,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2862,7 +2865,7 @@
         <v>29</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2872,12 +2875,12 @@
       <c r="C21" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G21" s="7"/>
     </row>
@@ -2895,7 +2898,7 @@
         <v>31</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2912,7 +2915,7 @@
         <v>33</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2929,7 +2932,7 @@
         <v>35</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2946,7 +2949,7 @@
         <v>37</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2963,7 +2966,7 @@
         <v>39</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2980,7 +2983,7 @@
         <v>41</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2990,12 +2993,12 @@
       <c r="C28" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G28" s="7"/>
     </row>
@@ -3013,7 +3016,7 @@
         <v>43</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3030,7 +3033,7 @@
         <v>45</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3047,7 +3050,7 @@
         <v>47</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3057,12 +3060,12 @@
       <c r="C32" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="E32" s="13"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G32" s="7"/>
     </row>
@@ -3080,7 +3083,7 @@
         <v>49</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3097,7 +3100,7 @@
         <v>51</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -3114,7 +3117,7 @@
         <v>53</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3131,7 +3134,7 @@
         <v>55</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3148,7 +3151,7 @@
         <v>57</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3163,7 +3166,7 @@
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G38" s="7"/>
     </row>
@@ -3174,12 +3177,12 @@
       <c r="C39" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="E39" s="13"/>
+      <c r="E39" s="14"/>
       <c r="F39" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G39" s="7"/>
     </row>
@@ -3197,7 +3200,7 @@
         <v>59</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3214,7 +3217,7 @@
         <v>61</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3231,7 +3234,7 @@
         <v>63</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3248,7 +3251,7 @@
         <v>65</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3265,7 +3268,7 @@
         <v>67</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3282,7 +3285,7 @@
         <v>69</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3299,7 +3302,7 @@
         <v>71</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3309,12 +3312,12 @@
       <c r="C47" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="E47" s="13"/>
+      <c r="E47" s="14"/>
       <c r="F47" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G47" s="7"/>
     </row>
@@ -3332,7 +3335,7 @@
         <v>73</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3349,7 +3352,7 @@
         <v>75</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3366,7 +3369,7 @@
         <v>77</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3383,7 +3386,7 @@
         <v>79</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3400,7 +3403,7 @@
         <v>81</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3410,12 +3413,12 @@
       <c r="C53" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="E53" s="13"/>
+      <c r="E53" s="14"/>
       <c r="F53" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G53" s="7"/>
     </row>
@@ -3433,7 +3436,7 @@
         <v>83</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3450,7 +3453,7 @@
         <v>85</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3467,7 +3470,7 @@
         <v>87</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3484,7 +3487,7 @@
         <v>89</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3501,7 +3504,7 @@
         <v>91</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3518,7 +3521,7 @@
         <v>93</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3535,7 +3538,7 @@
         <v>95</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3552,7 +3555,7 @@
         <v>97</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3562,12 +3565,12 @@
       <c r="C62" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="E62" s="13"/>
+      <c r="E62" s="14"/>
       <c r="F62" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G62" s="7"/>
     </row>
@@ -3585,7 +3588,7 @@
         <v>99</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3602,7 +3605,7 @@
         <v>101</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3619,7 +3622,7 @@
         <v>103</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3636,7 +3639,7 @@
         <v>105</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3653,7 +3656,7 @@
         <v>107</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3670,7 +3673,7 @@
         <v>109</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3687,7 +3690,7 @@
         <v>111</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3704,7 +3707,7 @@
         <v>113</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -3721,7 +3724,7 @@
         <v>115</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3738,7 +3741,7 @@
         <v>117</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3755,7 +3758,7 @@
         <v>119</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3772,7 +3775,7 @@
         <v>121</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3782,10 +3785,10 @@
       <c r="C75" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D75" s="13" t="s">
+      <c r="D75" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="E75" s="13"/>
+      <c r="E75" s="14"/>
       <c r="F75" s="2" t="s">
         <v>244</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>123</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3822,7 +3825,7 @@
         <v>125</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3832,12 +3835,12 @@
       <c r="C78" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D78" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="E78" s="13"/>
+      <c r="E78" s="14"/>
       <c r="F78" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G78" s="7"/>
     </row>
@@ -3855,7 +3858,7 @@
         <v>127</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3872,7 +3875,7 @@
         <v>129</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3889,7 +3892,7 @@
         <v>131</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3906,7 +3909,7 @@
         <v>133</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3923,7 +3926,7 @@
         <v>135</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3938,7 +3941,7 @@
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G84" s="7"/>
     </row>
@@ -3949,12 +3952,12 @@
       <c r="C85" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D85" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="E85" s="13"/>
+      <c r="E85" s="14"/>
       <c r="F85" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G85" s="7"/>
     </row>
@@ -3972,7 +3975,7 @@
         <v>137</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -3989,7 +3992,7 @@
         <v>139</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4006,7 +4009,7 @@
         <v>141</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4023,7 +4026,7 @@
         <v>143</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4040,7 +4043,7 @@
         <v>145</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4050,12 +4053,12 @@
       <c r="C91" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D91" s="13" t="s">
+      <c r="D91" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E91" s="13"/>
+      <c r="E91" s="14"/>
       <c r="F91" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G91" s="7"/>
     </row>
@@ -4073,7 +4076,7 @@
         <v>147</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4090,7 +4093,7 @@
         <v>149</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4107,7 +4110,7 @@
         <v>151</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4124,7 +4127,7 @@
         <v>153</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4141,7 +4144,7 @@
         <v>155</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4158,7 +4161,7 @@
         <v>157</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4175,7 +4178,7 @@
         <v>159</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4192,7 +4195,7 @@
         <v>161</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4202,12 +4205,12 @@
       <c r="C100" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D100" s="13" t="s">
+      <c r="D100" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="E100" s="13"/>
+      <c r="E100" s="14"/>
       <c r="F100" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G100" s="7"/>
     </row>
@@ -4225,7 +4228,7 @@
         <v>163</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4242,7 +4245,7 @@
         <v>165</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4259,7 +4262,7 @@
         <v>167</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4276,7 +4279,7 @@
         <v>169</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4293,7 +4296,7 @@
         <v>171</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4308,7 +4311,7 @@
       </c>
       <c r="E106" s="7"/>
       <c r="F106" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G106" s="7"/>
     </row>
@@ -4319,12 +4322,12 @@
       <c r="C107" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D107" s="13" t="s">
+      <c r="D107" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="E107" s="13"/>
+      <c r="E107" s="14"/>
       <c r="F107" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G107" s="7"/>
     </row>
@@ -4342,7 +4345,7 @@
         <v>173</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4352,10 +4355,10 @@
       <c r="C109" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D109" s="13" t="s">
+      <c r="D109" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="E109" s="13"/>
+      <c r="E109" s="14"/>
       <c r="F109" s="2" t="s">
         <v>266</v>
       </c>
@@ -4375,7 +4378,7 @@
         <v>175</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4392,7 +4395,7 @@
         <v>177</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4409,7 +4412,7 @@
         <v>179</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4426,7 +4429,7 @@
         <v>181</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4443,7 +4446,7 @@
         <v>183</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4454,12 +4457,12 @@
       <c r="C115" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D115" s="13" t="s">
+      <c r="D115" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="E115" s="13"/>
+      <c r="E115" s="14"/>
       <c r="F115" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G115" s="7"/>
     </row>
@@ -4477,7 +4480,7 @@
         <v>185</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4494,7 +4497,7 @@
         <v>187</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4511,7 +4514,7 @@
         <v>189</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4528,7 +4531,7 @@
         <v>191</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -4545,7 +4548,7 @@
         <v>193</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4556,12 +4559,12 @@
       <c r="C121" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D121" s="13" t="s">
+      <c r="D121" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="E121" s="13"/>
+      <c r="E121" s="14"/>
       <c r="F121" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G121" s="7"/>
     </row>
@@ -4579,7 +4582,7 @@
         <v>195</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4596,7 +4599,7 @@
         <v>197</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4613,7 +4616,7 @@
         <v>199</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4624,12 +4627,12 @@
       <c r="C125" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D125" s="13" t="s">
+      <c r="D125" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="E125" s="13"/>
+      <c r="E125" s="14"/>
       <c r="F125" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G125" s="7"/>
     </row>
@@ -4647,7 +4650,7 @@
         <v>201</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4664,7 +4667,7 @@
         <v>203</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4680,7 +4683,7 @@
       </c>
       <c r="E128" s="7"/>
       <c r="F128" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G128" s="7"/>
     </row>
@@ -4692,12 +4695,12 @@
       <c r="C129" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D129" s="13" t="s">
+      <c r="D129" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="E129" s="13"/>
+      <c r="E129" s="14"/>
       <c r="F129" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G129" s="7"/>
     </row>
@@ -4715,7 +4718,7 @@
         <v>205</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="131" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4726,12 +4729,12 @@
       <c r="C131" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D131" s="13" t="s">
+      <c r="D131" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="E131" s="13"/>
+      <c r="E131" s="14"/>
       <c r="F131" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G131" s="7"/>
     </row>
@@ -4749,7 +4752,7 @@
         <v>207</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4766,7 +4769,7 @@
         <v>209</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4777,10 +4780,10 @@
       <c r="C134" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D134" s="13" t="s">
+      <c r="D134" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="E134" s="13"/>
+      <c r="E134" s="14"/>
       <c r="F134" s="2" t="s">
         <v>266</v>
       </c>
@@ -4800,7 +4803,7 @@
         <v>211</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -4817,7 +4820,7 @@
         <v>213</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -4834,16 +4837,19 @@
         <v>215</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D125:E125"/>
     <mergeCell ref="D100:E100"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D39:E39"/>
@@ -4854,14 +4860,11 @@
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4911,10 +4914,10 @@
         <v>303</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -4928,10 +4931,10 @@
         <v>305</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -4945,10 +4948,10 @@
         <v>307</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -4962,10 +4965,10 @@
         <v>309</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>